<commit_message>
Update Wheat trait ontology
</commit_message>
<xml_diff>
--- a/ontology/triticum-props.xlsx
+++ b/ontology/triticum-props.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="565">
   <si>
     <t>trait_name</t>
   </si>
@@ -376,6 +376,12 @@
     <t>TRAIT: Plant height ::: METHOD: PH Measurement ::: SCALE: cm</t>
   </si>
   <si>
+    <t>Spike awnedness - 0-9 AWNS scale</t>
+  </si>
+  <si>
+    <t>TRAIT: Spike awnedness ::: METHOD: Awns Estimation ::: SCALE: 0-9 AWNS scale</t>
+  </si>
+  <si>
     <t>Spike length - cm</t>
   </si>
   <si>
@@ -463,6 +469,12 @@
     <t>TRAIT: Rachis length ::: METHOD: RachLng Measurement ::: SCALE: mm</t>
   </si>
   <si>
+    <t>Grain length - mm</t>
+  </si>
+  <si>
+    <t>TRAIT: Grain length ::: METHOD: GLng Measurement ::: SCALE: mm</t>
+  </si>
+  <si>
     <t>Grain width - mm</t>
   </si>
   <si>
@@ -1691,6 +1703,12 @@
   </si>
   <si>
     <t>TRAIT: Jointing time ::: METHOD: Jointing Time Measurement ::: SCALE: Julian date (JD)</t>
+  </si>
+  <si>
+    <t>Grain Area - mm2</t>
+  </si>
+  <si>
+    <t>TRAIT: Grain area ::: METHOD: Grain Area Computation ::: SCALE: mm2</t>
   </si>
 </sst>
 </file>
@@ -2022,7 +2040,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H265"/>
+  <dimension ref="A1:H268"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2872,13 +2890,10 @@
         <v>120</v>
       </c>
       <c r="B53" t="s">
-        <v>13</v>
-      </c>
-      <c r="D53">
-        <v>5</v>
-      </c>
-      <c r="E53">
-        <v>90</v>
+        <v>9</v>
+      </c>
+      <c r="F53" t="s">
+        <v>16</v>
       </c>
       <c r="G53" t="s">
         <v>121</v>
@@ -2892,10 +2907,10 @@
         <v>13</v>
       </c>
       <c r="D54">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E54">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="G54" t="s">
         <v>123</v>
@@ -2909,10 +2924,10 @@
         <v>13</v>
       </c>
       <c r="D55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E55">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G55" t="s">
         <v>125</v>
@@ -2923,10 +2938,13 @@
         <v>126</v>
       </c>
       <c r="B56" t="s">
-        <v>9</v>
-      </c>
-      <c r="F56" t="s">
-        <v>103</v>
+        <v>13</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>50</v>
       </c>
       <c r="G56" t="s">
         <v>127</v>
@@ -2937,13 +2955,10 @@
         <v>128</v>
       </c>
       <c r="B57" t="s">
-        <v>13</v>
-      </c>
-      <c r="D57">
-        <v>0</v>
-      </c>
-      <c r="E57">
-        <v>100</v>
+        <v>9</v>
+      </c>
+      <c r="F57" t="s">
+        <v>103</v>
       </c>
       <c r="G57" t="s">
         <v>129</v>
@@ -2971,27 +2986,27 @@
         <v>132</v>
       </c>
       <c r="B59" t="s">
-        <v>9</v>
-      </c>
-      <c r="F59" t="s">
+        <v>13</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>100</v>
+      </c>
+      <c r="G59" t="s">
         <v>133</v>
-      </c>
-      <c r="G59" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
+        <v>134</v>
+      </c>
+      <c r="B60" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" t="s">
         <v>135</v>
-      </c>
-      <c r="B60" t="s">
-        <v>13</v>
-      </c>
-      <c r="D60">
-        <v>0</v>
-      </c>
-      <c r="E60">
-        <v>100</v>
       </c>
       <c r="G60" t="s">
         <v>136</v>
@@ -3090,10 +3105,10 @@
         <v>13</v>
       </c>
       <c r="D66">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E66">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G66" t="s">
         <v>148</v>
@@ -3124,10 +3139,10 @@
         <v>13</v>
       </c>
       <c r="D68">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E68">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G68" t="s">
         <v>152</v>
@@ -3141,10 +3156,10 @@
         <v>13</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E69">
-        <v>1000</v>
+        <v>40</v>
       </c>
       <c r="G69" t="s">
         <v>154</v>
@@ -3158,10 +3173,10 @@
         <v>13</v>
       </c>
       <c r="D70">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E70">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="G70" t="s">
         <v>156</v>
@@ -3174,6 +3189,12 @@
       <c r="B71" t="s">
         <v>13</v>
       </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>1000</v>
+      </c>
       <c r="G71" t="s">
         <v>158</v>
       </c>
@@ -3186,10 +3207,10 @@
         <v>13</v>
       </c>
       <c r="D72">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E72">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="G72" t="s">
         <v>160</v>
@@ -3202,12 +3223,6 @@
       <c r="B73" t="s">
         <v>13</v>
       </c>
-      <c r="D73">
-        <v>1</v>
-      </c>
-      <c r="E73">
-        <v>15</v>
-      </c>
       <c r="G73" t="s">
         <v>162</v>
       </c>
@@ -3219,6 +3234,12 @@
       <c r="B74" t="s">
         <v>13</v>
       </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <v>15</v>
+      </c>
       <c r="G74" t="s">
         <v>164</v>
       </c>
@@ -3245,10 +3266,7 @@
         <v>167</v>
       </c>
       <c r="B76" t="s">
-        <v>9</v>
-      </c>
-      <c r="F76" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G76" t="s">
         <v>168</v>
@@ -3259,61 +3277,55 @@
         <v>169</v>
       </c>
       <c r="B77" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D77">
         <v>1</v>
       </c>
       <c r="E77">
-        <v>6</v>
-      </c>
-      <c r="F77" t="s">
+        <v>15</v>
+      </c>
+      <c r="G77" t="s">
         <v>170</v>
-      </c>
-      <c r="G77" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" t="s">
+        <v>171</v>
+      </c>
+      <c r="B78" t="s">
+        <v>9</v>
+      </c>
+      <c r="F78" t="s">
+        <v>16</v>
+      </c>
+      <c r="G78" t="s">
         <v>172</v>
-      </c>
-      <c r="B78" t="s">
-        <v>13</v>
-      </c>
-      <c r="D78">
-        <v>0</v>
-      </c>
-      <c r="E78">
-        <v>100</v>
-      </c>
-      <c r="G78" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" t="s">
+        <v>173</v>
+      </c>
+      <c r="B79" t="s">
+        <v>9</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <v>6</v>
+      </c>
+      <c r="F79" t="s">
         <v>174</v>
       </c>
-      <c r="B79" t="s">
-        <v>9</v>
-      </c>
-      <c r="D79">
-        <v>0</v>
-      </c>
-      <c r="E79">
-        <v>10</v>
-      </c>
-      <c r="F79" t="s">
+      <c r="G79" t="s">
         <v>175</v>
-      </c>
-      <c r="G79" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B80" t="s">
         <v>13</v>
@@ -3325,24 +3337,24 @@
         <v>100</v>
       </c>
       <c r="G80" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" t="s">
+        <v>178</v>
+      </c>
+      <c r="B81" t="s">
+        <v>9</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>10</v>
+      </c>
+      <c r="F81" t="s">
         <v>179</v>
-      </c>
-      <c r="B81" t="s">
-        <v>9</v>
-      </c>
-      <c r="D81">
-        <v>1</v>
-      </c>
-      <c r="E81">
-        <v>9</v>
-      </c>
-      <c r="F81" t="s">
-        <v>103</v>
       </c>
       <c r="G81" t="s">
         <v>180</v>
@@ -3356,10 +3368,10 @@
         <v>13</v>
       </c>
       <c r="D82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E82">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="G82" t="s">
         <v>182</v>
@@ -3370,13 +3382,16 @@
         <v>183</v>
       </c>
       <c r="B83" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E83">
-        <v>100</v>
+        <v>9</v>
+      </c>
+      <c r="F83" t="s">
+        <v>103</v>
       </c>
       <c r="G83" t="s">
         <v>184</v>
@@ -3389,6 +3404,12 @@
       <c r="B84" t="s">
         <v>13</v>
       </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="E84">
+        <v>15</v>
+      </c>
       <c r="G84" t="s">
         <v>186</v>
       </c>
@@ -3400,6 +3421,12 @@
       <c r="B85" t="s">
         <v>13</v>
       </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>100</v>
+      </c>
       <c r="G85" t="s">
         <v>188</v>
       </c>
@@ -3433,12 +3460,6 @@
       <c r="B88" t="s">
         <v>13</v>
       </c>
-      <c r="D88">
-        <v>1</v>
-      </c>
-      <c r="E88">
-        <v>15</v>
-      </c>
       <c r="G88" t="s">
         <v>194</v>
       </c>
@@ -3450,12 +3471,6 @@
       <c r="B89" t="s">
         <v>13</v>
       </c>
-      <c r="D89">
-        <v>1</v>
-      </c>
-      <c r="E89">
-        <v>15</v>
-      </c>
       <c r="G89" t="s">
         <v>196</v>
       </c>
@@ -3468,10 +3483,10 @@
         <v>13</v>
       </c>
       <c r="D90">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E90">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="G90" t="s">
         <v>198</v>
@@ -3485,10 +3500,10 @@
         <v>13</v>
       </c>
       <c r="D91">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E91">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G91" t="s">
         <v>200</v>
@@ -3502,10 +3517,10 @@
         <v>13</v>
       </c>
       <c r="D92">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E92">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="G92" t="s">
         <v>202</v>
@@ -3519,10 +3534,10 @@
         <v>13</v>
       </c>
       <c r="D93">
-        <v>40</v>
+        <v>-1</v>
       </c>
       <c r="E93">
-        <v>240</v>
+        <v>1</v>
       </c>
       <c r="G93" t="s">
         <v>204</v>
@@ -3539,7 +3554,7 @@
         <v>1</v>
       </c>
       <c r="E94">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="G94" t="s">
         <v>206</v>
@@ -3553,10 +3568,10 @@
         <v>13</v>
       </c>
       <c r="D95">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E95">
-        <v>100</v>
+        <v>240</v>
       </c>
       <c r="G95" t="s">
         <v>208</v>
@@ -3570,10 +3585,10 @@
         <v>13</v>
       </c>
       <c r="D96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E96">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G96" t="s">
         <v>210</v>
@@ -3618,16 +3633,13 @@
         <v>215</v>
       </c>
       <c r="B99" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E99">
-        <v>9</v>
-      </c>
-      <c r="F99" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G99" t="s">
         <v>216</v>
@@ -3638,16 +3650,13 @@
         <v>217</v>
       </c>
       <c r="B100" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E100">
-        <v>9</v>
-      </c>
-      <c r="F100" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G100" t="s">
         <v>218</v>
@@ -3658,7 +3667,16 @@
         <v>219</v>
       </c>
       <c r="B101" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="D101">
+        <v>1</v>
+      </c>
+      <c r="E101">
+        <v>9</v>
+      </c>
+      <c r="F101" t="s">
+        <v>103</v>
       </c>
       <c r="G101" t="s">
         <v>220</v>
@@ -3672,13 +3690,13 @@
         <v>9</v>
       </c>
       <c r="D102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E102">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F102" t="s">
-        <v>175</v>
+        <v>103</v>
       </c>
       <c r="G102" t="s">
         <v>222</v>
@@ -3689,10 +3707,7 @@
         <v>223</v>
       </c>
       <c r="B103" t="s">
-        <v>9</v>
-      </c>
-      <c r="F103" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G103" t="s">
         <v>224</v>
@@ -3703,13 +3718,16 @@
         <v>225</v>
       </c>
       <c r="B104" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D104">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E104">
-        <v>240</v>
+        <v>10</v>
+      </c>
+      <c r="F104" t="s">
+        <v>179</v>
       </c>
       <c r="G104" t="s">
         <v>226</v>
@@ -3720,13 +3738,10 @@
         <v>227</v>
       </c>
       <c r="B105" t="s">
-        <v>13</v>
-      </c>
-      <c r="D105">
-        <v>5</v>
-      </c>
-      <c r="E105">
-        <v>90</v>
+        <v>9</v>
+      </c>
+      <c r="F105" t="s">
+        <v>16</v>
       </c>
       <c r="G105" t="s">
         <v>228</v>
@@ -3740,10 +3755,10 @@
         <v>13</v>
       </c>
       <c r="D106">
-        <v>-1</v>
+        <v>40</v>
       </c>
       <c r="E106">
-        <v>1</v>
+        <v>240</v>
       </c>
       <c r="G106" t="s">
         <v>230</v>
@@ -3754,7 +3769,13 @@
         <v>231</v>
       </c>
       <c r="B107" t="s">
-        <v>94</v>
+        <v>13</v>
+      </c>
+      <c r="D107">
+        <v>5</v>
+      </c>
+      <c r="E107">
+        <v>90</v>
       </c>
       <c r="G107" t="s">
         <v>232</v>
@@ -3768,10 +3789,10 @@
         <v>13</v>
       </c>
       <c r="D108">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E108">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G108" t="s">
         <v>234</v>
@@ -3782,13 +3803,7 @@
         <v>235</v>
       </c>
       <c r="B109" t="s">
-        <v>13</v>
-      </c>
-      <c r="D109">
-        <v>0</v>
-      </c>
-      <c r="E109">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G109" t="s">
         <v>236</v>
@@ -3873,7 +3888,7 @@
         <v>0</v>
       </c>
       <c r="E114">
-        <v>20000</v>
+        <v>100</v>
       </c>
       <c r="G114" t="s">
         <v>246</v>
@@ -3884,58 +3899,70 @@
         <v>247</v>
       </c>
       <c r="B115" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D115">
         <v>0</v>
       </c>
       <c r="E115">
-        <v>3</v>
-      </c>
-      <c r="F115" t="s">
+        <v>100</v>
+      </c>
+      <c r="G115" t="s">
         <v>248</v>
-      </c>
-      <c r="G115" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="116" spans="1:7">
       <c r="A116" t="s">
+        <v>249</v>
+      </c>
+      <c r="B116" t="s">
+        <v>13</v>
+      </c>
+      <c r="D116">
+        <v>0</v>
+      </c>
+      <c r="E116">
+        <v>20000</v>
+      </c>
+      <c r="G116" t="s">
         <v>250</v>
-      </c>
-      <c r="B116" t="s">
-        <v>9</v>
-      </c>
-      <c r="D116">
-        <v>0</v>
-      </c>
-      <c r="E116">
-        <v>1</v>
-      </c>
-      <c r="F116" t="s">
-        <v>251</v>
-      </c>
-      <c r="G116" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="117" spans="1:7">
       <c r="A117" t="s">
+        <v>251</v>
+      </c>
+      <c r="B117" t="s">
+        <v>9</v>
+      </c>
+      <c r="D117">
+        <v>0</v>
+      </c>
+      <c r="E117">
+        <v>3</v>
+      </c>
+      <c r="F117" t="s">
+        <v>252</v>
+      </c>
+      <c r="G117" t="s">
         <v>253</v>
-      </c>
-      <c r="B117" t="s">
-        <v>13</v>
-      </c>
-      <c r="G117" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="118" spans="1:7">
       <c r="A118" t="s">
+        <v>254</v>
+      </c>
+      <c r="B118" t="s">
+        <v>9</v>
+      </c>
+      <c r="D118">
+        <v>0</v>
+      </c>
+      <c r="E118">
+        <v>1</v>
+      </c>
+      <c r="F118" t="s">
         <v>255</v>
-      </c>
-      <c r="B118" t="s">
-        <v>13</v>
       </c>
       <c r="G118" t="s">
         <v>256</v>
@@ -3959,12 +3986,6 @@
       <c r="B120" t="s">
         <v>13</v>
       </c>
-      <c r="D120">
-        <v>0</v>
-      </c>
-      <c r="E120">
-        <v>20000</v>
-      </c>
       <c r="G120" t="s">
         <v>260</v>
       </c>
@@ -3974,50 +3995,44 @@
         <v>261</v>
       </c>
       <c r="B121" t="s">
-        <v>9</v>
-      </c>
-      <c r="D121">
-        <v>1</v>
-      </c>
-      <c r="E121">
-        <v>4</v>
-      </c>
-      <c r="F121" t="s">
+        <v>13</v>
+      </c>
+      <c r="G121" t="s">
         <v>262</v>
-      </c>
-      <c r="G121" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="122" spans="1:7">
       <c r="A122" t="s">
+        <v>263</v>
+      </c>
+      <c r="B122" t="s">
+        <v>13</v>
+      </c>
+      <c r="D122">
+        <v>0</v>
+      </c>
+      <c r="E122">
+        <v>20000</v>
+      </c>
+      <c r="G122" t="s">
         <v>264</v>
-      </c>
-      <c r="B122" t="s">
-        <v>9</v>
-      </c>
-      <c r="D122">
-        <v>0</v>
-      </c>
-      <c r="E122">
-        <v>1</v>
-      </c>
-      <c r="F122" t="s">
-        <v>251</v>
-      </c>
-      <c r="G122" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="123" spans="1:7">
       <c r="A123" t="s">
+        <v>265</v>
+      </c>
+      <c r="B123" t="s">
+        <v>9</v>
+      </c>
+      <c r="D123">
+        <v>1</v>
+      </c>
+      <c r="E123">
+        <v>4</v>
+      </c>
+      <c r="F123" t="s">
         <v>266</v>
-      </c>
-      <c r="B123" t="s">
-        <v>9</v>
-      </c>
-      <c r="F123" t="s">
-        <v>16</v>
       </c>
       <c r="G123" t="s">
         <v>267</v>
@@ -4030,8 +4045,14 @@
       <c r="B124" t="s">
         <v>9</v>
       </c>
+      <c r="D124">
+        <v>0</v>
+      </c>
+      <c r="E124">
+        <v>1</v>
+      </c>
       <c r="F124" t="s">
-        <v>16</v>
+        <v>255</v>
       </c>
       <c r="G124" t="s">
         <v>269</v>
@@ -4086,14 +4107,8 @@
       <c r="B128" t="s">
         <v>9</v>
       </c>
-      <c r="D128">
-        <v>1</v>
-      </c>
-      <c r="E128">
-        <v>9</v>
-      </c>
       <c r="F128" t="s">
-        <v>103</v>
+        <v>16</v>
       </c>
       <c r="G128" t="s">
         <v>277</v>
@@ -4104,13 +4119,10 @@
         <v>278</v>
       </c>
       <c r="B129" t="s">
-        <v>13</v>
-      </c>
-      <c r="D129">
-        <v>1</v>
-      </c>
-      <c r="E129">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="F129" t="s">
+        <v>16</v>
       </c>
       <c r="G129" t="s">
         <v>279</v>
@@ -4121,13 +4133,16 @@
         <v>280</v>
       </c>
       <c r="B130" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D130">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E130">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="F130" t="s">
+        <v>103</v>
       </c>
       <c r="G130" t="s">
         <v>281</v>
@@ -4141,10 +4156,10 @@
         <v>13</v>
       </c>
       <c r="D131">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E131">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="G131" t="s">
         <v>283</v>
@@ -4157,6 +4172,12 @@
       <c r="B132" t="s">
         <v>13</v>
       </c>
+      <c r="D132">
+        <v>-1</v>
+      </c>
+      <c r="E132">
+        <v>1</v>
+      </c>
       <c r="G132" t="s">
         <v>285</v>
       </c>
@@ -4166,10 +4187,13 @@
         <v>286</v>
       </c>
       <c r="B133" t="s">
-        <v>9</v>
-      </c>
-      <c r="F133" t="s">
-        <v>133</v>
+        <v>13</v>
+      </c>
+      <c r="D133">
+        <v>0</v>
+      </c>
+      <c r="E133">
+        <v>100</v>
       </c>
       <c r="G133" t="s">
         <v>287</v>
@@ -4180,38 +4204,35 @@
         <v>288</v>
       </c>
       <c r="B134" t="s">
-        <v>9</v>
-      </c>
-      <c r="F134" t="s">
+        <v>13</v>
+      </c>
+      <c r="G134" t="s">
         <v>289</v>
-      </c>
-      <c r="G134" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="135" spans="1:7">
       <c r="A135" t="s">
+        <v>290</v>
+      </c>
+      <c r="B135" t="s">
+        <v>9</v>
+      </c>
+      <c r="F135" t="s">
+        <v>135</v>
+      </c>
+      <c r="G135" t="s">
         <v>291</v>
-      </c>
-      <c r="B135" t="s">
-        <v>9</v>
-      </c>
-      <c r="F135" t="s">
-        <v>133</v>
-      </c>
-      <c r="G135" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="136" spans="1:7">
       <c r="A136" t="s">
+        <v>292</v>
+      </c>
+      <c r="B136" t="s">
+        <v>9</v>
+      </c>
+      <c r="F136" t="s">
         <v>293</v>
-      </c>
-      <c r="B136" t="s">
-        <v>9</v>
-      </c>
-      <c r="F136" t="s">
-        <v>133</v>
       </c>
       <c r="G136" t="s">
         <v>294</v>
@@ -4225,7 +4246,7 @@
         <v>9</v>
       </c>
       <c r="F137" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G137" t="s">
         <v>296</v>
@@ -4236,13 +4257,10 @@
         <v>297</v>
       </c>
       <c r="B138" t="s">
-        <v>13</v>
-      </c>
-      <c r="D138">
-        <v>0</v>
-      </c>
-      <c r="E138">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="F138" t="s">
+        <v>135</v>
       </c>
       <c r="G138" t="s">
         <v>298</v>
@@ -4253,13 +4271,10 @@
         <v>299</v>
       </c>
       <c r="B139" t="s">
-        <v>13</v>
-      </c>
-      <c r="D139">
-        <v>1</v>
-      </c>
-      <c r="E139">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="F139" t="s">
+        <v>135</v>
       </c>
       <c r="G139" t="s">
         <v>300</v>
@@ -4276,7 +4291,7 @@
         <v>0</v>
       </c>
       <c r="E140">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G140" t="s">
         <v>302</v>
@@ -4290,10 +4305,10 @@
         <v>13</v>
       </c>
       <c r="D141">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E141">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="G141" t="s">
         <v>304</v>
@@ -4304,7 +4319,13 @@
         <v>305</v>
       </c>
       <c r="B142" t="s">
-        <v>94</v>
+        <v>13</v>
+      </c>
+      <c r="D142">
+        <v>0</v>
+      </c>
+      <c r="E142">
+        <v>100</v>
       </c>
       <c r="G142" t="s">
         <v>306</v>
@@ -4315,7 +4336,13 @@
         <v>307</v>
       </c>
       <c r="B143" t="s">
-        <v>94</v>
+        <v>13</v>
+      </c>
+      <c r="D143">
+        <v>0</v>
+      </c>
+      <c r="E143">
+        <v>100</v>
       </c>
       <c r="G143" t="s">
         <v>308</v>
@@ -4326,13 +4353,7 @@
         <v>309</v>
       </c>
       <c r="B144" t="s">
-        <v>13</v>
-      </c>
-      <c r="D144">
-        <v>1</v>
-      </c>
-      <c r="E144">
-        <v>15</v>
+        <v>94</v>
       </c>
       <c r="G144" t="s">
         <v>310</v>
@@ -4343,7 +4364,7 @@
         <v>311</v>
       </c>
       <c r="B145" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="G145" t="s">
         <v>312</v>
@@ -4354,16 +4375,13 @@
         <v>313</v>
       </c>
       <c r="B146" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D146">
         <v>1</v>
       </c>
       <c r="E146">
-        <v>6</v>
-      </c>
-      <c r="F146" t="s">
-        <v>170</v>
+        <v>15</v>
       </c>
       <c r="G146" t="s">
         <v>314</v>
@@ -4376,12 +4394,6 @@
       <c r="B147" t="s">
         <v>13</v>
       </c>
-      <c r="D147">
-        <v>0</v>
-      </c>
-      <c r="E147">
-        <v>100</v>
-      </c>
       <c r="G147" t="s">
         <v>316</v>
       </c>
@@ -4391,13 +4403,16 @@
         <v>317</v>
       </c>
       <c r="B148" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D148">
         <v>1</v>
       </c>
       <c r="E148">
-        <v>15</v>
+        <v>6</v>
+      </c>
+      <c r="F148" t="s">
+        <v>174</v>
       </c>
       <c r="G148" t="s">
         <v>318</v>
@@ -4411,10 +4426,10 @@
         <v>13</v>
       </c>
       <c r="D149">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E149">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="G149" t="s">
         <v>320</v>
@@ -4425,16 +4440,13 @@
         <v>321</v>
       </c>
       <c r="B150" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D150">
         <v>1</v>
       </c>
       <c r="E150">
-        <v>6</v>
-      </c>
-      <c r="F150" t="s">
-        <v>170</v>
+        <v>15</v>
       </c>
       <c r="G150" t="s">
         <v>322</v>
@@ -4448,10 +4460,10 @@
         <v>13</v>
       </c>
       <c r="D151">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E151">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="G151" t="s">
         <v>324</v>
@@ -4462,13 +4474,16 @@
         <v>325</v>
       </c>
       <c r="B152" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D152">
         <v>1</v>
       </c>
       <c r="E152">
-        <v>15</v>
+        <v>6</v>
+      </c>
+      <c r="F152" t="s">
+        <v>174</v>
       </c>
       <c r="G152" t="s">
         <v>326</v>
@@ -4482,10 +4497,10 @@
         <v>13</v>
       </c>
       <c r="D153">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E153">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="G153" t="s">
         <v>328</v>
@@ -4513,16 +4528,13 @@
         <v>331</v>
       </c>
       <c r="B155" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D155">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E155">
-        <v>4</v>
-      </c>
-      <c r="F155" t="s">
-        <v>289</v>
+        <v>15</v>
       </c>
       <c r="G155" t="s">
         <v>332</v>
@@ -4536,10 +4548,10 @@
         <v>13</v>
       </c>
       <c r="D156">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E156">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G156" t="s">
         <v>334</v>
@@ -4556,10 +4568,10 @@
         <v>0</v>
       </c>
       <c r="E157">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F157" t="s">
-        <v>175</v>
+        <v>293</v>
       </c>
       <c r="G157" t="s">
         <v>336</v>
@@ -4570,16 +4582,13 @@
         <v>337</v>
       </c>
       <c r="B158" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D158">
         <v>0</v>
       </c>
       <c r="E158">
         <v>1</v>
-      </c>
-      <c r="F158" t="s">
-        <v>251</v>
       </c>
       <c r="G158" t="s">
         <v>338</v>
@@ -4590,13 +4599,16 @@
         <v>339</v>
       </c>
       <c r="B159" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D159">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E159">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="F159" t="s">
+        <v>179</v>
       </c>
       <c r="G159" t="s">
         <v>340</v>
@@ -4607,7 +4619,16 @@
         <v>341</v>
       </c>
       <c r="B160" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="D160">
+        <v>0</v>
+      </c>
+      <c r="E160">
+        <v>1</v>
+      </c>
+      <c r="F160" t="s">
+        <v>255</v>
       </c>
       <c r="G160" t="s">
         <v>342</v>
@@ -4621,10 +4642,10 @@
         <v>13</v>
       </c>
       <c r="D161">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E161">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G161" t="s">
         <v>344</v>
@@ -4637,12 +4658,6 @@
       <c r="B162" t="s">
         <v>13</v>
       </c>
-      <c r="D162">
-        <v>0</v>
-      </c>
-      <c r="E162">
-        <v>100</v>
-      </c>
       <c r="G162" t="s">
         <v>346</v>
       </c>
@@ -4652,16 +4667,13 @@
         <v>347</v>
       </c>
       <c r="B163" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D163">
+        <v>-1</v>
+      </c>
+      <c r="E163">
         <v>1</v>
-      </c>
-      <c r="E163">
-        <v>5</v>
-      </c>
-      <c r="F163" t="s">
-        <v>10</v>
       </c>
       <c r="G163" t="s">
         <v>348</v>
@@ -4672,10 +4684,13 @@
         <v>349</v>
       </c>
       <c r="B164" t="s">
-        <v>9</v>
-      </c>
-      <c r="F164" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="D164">
+        <v>0</v>
+      </c>
+      <c r="E164">
+        <v>100</v>
       </c>
       <c r="G164" t="s">
         <v>350</v>
@@ -4686,7 +4701,16 @@
         <v>351</v>
       </c>
       <c r="B165" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="D165">
+        <v>1</v>
+      </c>
+      <c r="E165">
+        <v>5</v>
+      </c>
+      <c r="F165" t="s">
+        <v>10</v>
       </c>
       <c r="G165" t="s">
         <v>352</v>
@@ -4711,10 +4735,7 @@
         <v>355</v>
       </c>
       <c r="B167" t="s">
-        <v>9</v>
-      </c>
-      <c r="F167" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G167" t="s">
         <v>356</v>
@@ -4755,14 +4776,8 @@
       <c r="B170" t="s">
         <v>9</v>
       </c>
-      <c r="D170">
-        <v>1</v>
-      </c>
-      <c r="E170">
-        <v>9</v>
-      </c>
       <c r="F170" t="s">
-        <v>103</v>
+        <v>16</v>
       </c>
       <c r="G170" t="s">
         <v>362</v>
@@ -4773,13 +4788,10 @@
         <v>363</v>
       </c>
       <c r="B171" t="s">
-        <v>13</v>
-      </c>
-      <c r="D171">
-        <v>0</v>
-      </c>
-      <c r="E171">
-        <v>100</v>
+        <v>9</v>
+      </c>
+      <c r="F171" t="s">
+        <v>16</v>
       </c>
       <c r="G171" t="s">
         <v>364</v>
@@ -4790,13 +4802,16 @@
         <v>365</v>
       </c>
       <c r="B172" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D172">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E172">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="F172" t="s">
+        <v>103</v>
       </c>
       <c r="G172" t="s">
         <v>366</v>
@@ -4813,10 +4828,7 @@
         <v>0</v>
       </c>
       <c r="E173">
-        <v>9</v>
-      </c>
-      <c r="F173" t="s">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="G173" t="s">
         <v>368</v>
@@ -4833,10 +4845,7 @@
         <v>0</v>
       </c>
       <c r="E174">
-        <v>9</v>
-      </c>
-      <c r="F174" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G174" t="s">
         <v>370</v>
@@ -4927,6 +4936,12 @@
         <v>379</v>
       </c>
       <c r="B179" t="s">
+        <v>13</v>
+      </c>
+      <c r="D179">
+        <v>0</v>
+      </c>
+      <c r="E179">
         <v>9</v>
       </c>
       <c r="F179" t="s">
@@ -4941,50 +4956,50 @@
         <v>381</v>
       </c>
       <c r="B180" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D180">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E180">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="F180" t="s">
+        <v>16</v>
+      </c>
+      <c r="G180" t="s">
         <v>382</v>
-      </c>
-      <c r="G180" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="181" spans="1:7">
       <c r="A181" t="s">
+        <v>383</v>
+      </c>
+      <c r="B181" t="s">
+        <v>9</v>
+      </c>
+      <c r="F181" t="s">
+        <v>16</v>
+      </c>
+      <c r="G181" t="s">
         <v>384</v>
-      </c>
-      <c r="B181" t="s">
-        <v>13</v>
-      </c>
-      <c r="D181">
-        <v>-1</v>
-      </c>
-      <c r="E181">
-        <v>1</v>
-      </c>
-      <c r="G181" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="182" spans="1:7">
       <c r="A182" t="s">
+        <v>385</v>
+      </c>
+      <c r="B182" t="s">
+        <v>9</v>
+      </c>
+      <c r="D182">
+        <v>5</v>
+      </c>
+      <c r="E182">
+        <v>25</v>
+      </c>
+      <c r="F182" t="s">
         <v>386</v>
-      </c>
-      <c r="B182" t="s">
-        <v>13</v>
-      </c>
-      <c r="D182">
-        <v>0</v>
-      </c>
-      <c r="E182">
-        <v>100</v>
       </c>
       <c r="G182" t="s">
         <v>387</v>
@@ -4997,6 +5012,12 @@
       <c r="B183" t="s">
         <v>13</v>
       </c>
+      <c r="D183">
+        <v>-1</v>
+      </c>
+      <c r="E183">
+        <v>1</v>
+      </c>
       <c r="G183" t="s">
         <v>389</v>
       </c>
@@ -5023,16 +5044,7 @@
         <v>392</v>
       </c>
       <c r="B185" t="s">
-        <v>9</v>
-      </c>
-      <c r="D185">
-        <v>1</v>
-      </c>
-      <c r="E185">
-        <v>9</v>
-      </c>
-      <c r="F185" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="G185" t="s">
         <v>393</v>
@@ -5043,16 +5055,13 @@
         <v>394</v>
       </c>
       <c r="B186" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D186">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E186">
-        <v>9</v>
-      </c>
-      <c r="F186" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G186" t="s">
         <v>395</v>
@@ -5063,13 +5072,16 @@
         <v>396</v>
       </c>
       <c r="B187" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D187">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E187">
-        <v>100</v>
+        <v>9</v>
+      </c>
+      <c r="F187" t="s">
+        <v>103</v>
       </c>
       <c r="G187" t="s">
         <v>397</v>
@@ -5080,13 +5092,16 @@
         <v>398</v>
       </c>
       <c r="B188" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D188">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E188">
-        <v>100</v>
+        <v>9</v>
+      </c>
+      <c r="F188" t="s">
+        <v>103</v>
       </c>
       <c r="G188" t="s">
         <v>399</v>
@@ -5097,50 +5112,50 @@
         <v>400</v>
       </c>
       <c r="B189" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D189">
         <v>0</v>
       </c>
       <c r="E189">
-        <v>5</v>
-      </c>
-      <c r="F189" t="s">
+        <v>100</v>
+      </c>
+      <c r="G189" t="s">
         <v>401</v>
-      </c>
-      <c r="G189" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="190" spans="1:7">
       <c r="A190" t="s">
+        <v>402</v>
+      </c>
+      <c r="B190" t="s">
+        <v>13</v>
+      </c>
+      <c r="D190">
+        <v>0</v>
+      </c>
+      <c r="E190">
+        <v>100</v>
+      </c>
+      <c r="G190" t="s">
         <v>403</v>
-      </c>
-      <c r="B190" t="s">
-        <v>9</v>
-      </c>
-      <c r="D190">
-        <v>0</v>
-      </c>
-      <c r="E190">
-        <v>9</v>
-      </c>
-      <c r="F190" t="s">
-        <v>16</v>
-      </c>
-      <c r="G190" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="191" spans="1:7">
       <c r="A191" t="s">
+        <v>404</v>
+      </c>
+      <c r="B191" t="s">
+        <v>9</v>
+      </c>
+      <c r="D191">
+        <v>0</v>
+      </c>
+      <c r="E191">
+        <v>5</v>
+      </c>
+      <c r="F191" t="s">
         <v>405</v>
-      </c>
-      <c r="B191" t="s">
-        <v>9</v>
-      </c>
-      <c r="F191" t="s">
-        <v>133</v>
       </c>
       <c r="G191" t="s">
         <v>406</v>
@@ -5151,7 +5166,16 @@
         <v>407</v>
       </c>
       <c r="B192" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="D192">
+        <v>0</v>
+      </c>
+      <c r="E192">
+        <v>9</v>
+      </c>
+      <c r="F192" t="s">
+        <v>16</v>
       </c>
       <c r="G192" t="s">
         <v>408</v>
@@ -5162,7 +5186,10 @@
         <v>409</v>
       </c>
       <c r="B193" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="F193" t="s">
+        <v>135</v>
       </c>
       <c r="G193" t="s">
         <v>410</v>
@@ -5208,12 +5235,6 @@
       <c r="B197" t="s">
         <v>13</v>
       </c>
-      <c r="D197">
-        <v>0</v>
-      </c>
-      <c r="E197">
-        <v>100</v>
-      </c>
       <c r="G197" t="s">
         <v>418</v>
       </c>
@@ -5223,10 +5244,7 @@
         <v>419</v>
       </c>
       <c r="B198" t="s">
-        <v>9</v>
-      </c>
-      <c r="F198" t="s">
-        <v>262</v>
+        <v>13</v>
       </c>
       <c r="G198" t="s">
         <v>420</v>
@@ -5237,10 +5255,13 @@
         <v>421</v>
       </c>
       <c r="B199" t="s">
-        <v>9</v>
-      </c>
-      <c r="F199" t="s">
-        <v>170</v>
+        <v>13</v>
+      </c>
+      <c r="D199">
+        <v>0</v>
+      </c>
+      <c r="E199">
+        <v>100</v>
       </c>
       <c r="G199" t="s">
         <v>422</v>
@@ -5254,7 +5275,7 @@
         <v>9</v>
       </c>
       <c r="F200" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="G200" t="s">
         <v>424</v>
@@ -5265,16 +5286,10 @@
         <v>425</v>
       </c>
       <c r="B201" t="s">
-        <v>13</v>
-      </c>
-      <c r="D201">
-        <v>0</v>
-      </c>
-      <c r="E201">
         <v>9</v>
       </c>
       <c r="F201" t="s">
-        <v>16</v>
+        <v>174</v>
       </c>
       <c r="G201" t="s">
         <v>426</v>
@@ -5287,14 +5302,8 @@
       <c r="B202" t="s">
         <v>9</v>
       </c>
-      <c r="D202">
-        <v>0</v>
-      </c>
-      <c r="E202">
-        <v>9</v>
-      </c>
       <c r="F202" t="s">
-        <v>16</v>
+        <v>266</v>
       </c>
       <c r="G202" t="s">
         <v>428</v>
@@ -5311,7 +5320,10 @@
         <v>0</v>
       </c>
       <c r="E203">
-        <v>100</v>
+        <v>9</v>
+      </c>
+      <c r="F203" t="s">
+        <v>16</v>
       </c>
       <c r="G203" t="s">
         <v>430</v>
@@ -5325,13 +5337,13 @@
         <v>9</v>
       </c>
       <c r="D204">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E204">
         <v>9</v>
       </c>
       <c r="F204" t="s">
-        <v>103</v>
+        <v>16</v>
       </c>
       <c r="G204" t="s">
         <v>432</v>
@@ -5359,13 +5371,16 @@
         <v>435</v>
       </c>
       <c r="B206" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D206">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E206">
-        <v>2.5</v>
+        <v>9</v>
+      </c>
+      <c r="F206" t="s">
+        <v>103</v>
       </c>
       <c r="G206" t="s">
         <v>436</v>
@@ -5378,6 +5393,12 @@
       <c r="B207" t="s">
         <v>13</v>
       </c>
+      <c r="D207">
+        <v>0</v>
+      </c>
+      <c r="E207">
+        <v>100</v>
+      </c>
       <c r="G207" t="s">
         <v>438</v>
       </c>
@@ -5393,7 +5414,7 @@
         <v>0</v>
       </c>
       <c r="E208">
-        <v>1000</v>
+        <v>2.5</v>
       </c>
       <c r="G208" t="s">
         <v>440</v>
@@ -5501,6 +5522,12 @@
       <c r="B216" t="s">
         <v>13</v>
       </c>
+      <c r="D216">
+        <v>0</v>
+      </c>
+      <c r="E216">
+        <v>1000</v>
+      </c>
       <c r="G216" t="s">
         <v>456</v>
       </c>
@@ -5512,12 +5539,6 @@
       <c r="B217" t="s">
         <v>13</v>
       </c>
-      <c r="D217">
-        <v>0</v>
-      </c>
-      <c r="E217">
-        <v>100</v>
-      </c>
       <c r="G217" t="s">
         <v>458</v>
       </c>
@@ -5540,6 +5561,12 @@
       <c r="B219" t="s">
         <v>13</v>
       </c>
+      <c r="D219">
+        <v>0</v>
+      </c>
+      <c r="E219">
+        <v>100</v>
+      </c>
       <c r="G219" t="s">
         <v>462</v>
       </c>
@@ -5549,10 +5576,7 @@
         <v>463</v>
       </c>
       <c r="B220" t="s">
-        <v>9</v>
-      </c>
-      <c r="F220" t="s">
-        <v>262</v>
+        <v>13</v>
       </c>
       <c r="G220" t="s">
         <v>464</v>
@@ -5574,7 +5598,10 @@
         <v>467</v>
       </c>
       <c r="B222" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="F222" t="s">
+        <v>266</v>
       </c>
       <c r="G222" t="s">
         <v>468</v>
@@ -5651,7 +5678,7 @@
         <v>481</v>
       </c>
       <c r="B229" t="s">
-        <v>94</v>
+        <v>13</v>
       </c>
       <c r="G229" t="s">
         <v>482</v>
@@ -5662,10 +5689,7 @@
         <v>483</v>
       </c>
       <c r="B230" t="s">
-        <v>9</v>
-      </c>
-      <c r="F230" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G230" t="s">
         <v>484</v>
@@ -5676,66 +5700,69 @@
         <v>485</v>
       </c>
       <c r="B231" t="s">
-        <v>9</v>
-      </c>
-      <c r="F231" t="s">
+        <v>94</v>
+      </c>
+      <c r="G231" t="s">
         <v>486</v>
-      </c>
-      <c r="G231" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="232" spans="1:7">
       <c r="A232" t="s">
+        <v>487</v>
+      </c>
+      <c r="B232" t="s">
+        <v>9</v>
+      </c>
+      <c r="F232" t="s">
+        <v>10</v>
+      </c>
+      <c r="G232" t="s">
         <v>488</v>
-      </c>
-      <c r="B232" t="s">
-        <v>9</v>
-      </c>
-      <c r="F232" t="s">
-        <v>486</v>
-      </c>
-      <c r="G232" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="233" spans="1:7">
       <c r="A233" t="s">
+        <v>489</v>
+      </c>
+      <c r="B233" t="s">
+        <v>9</v>
+      </c>
+      <c r="F233" t="s">
         <v>490</v>
       </c>
-      <c r="B233" t="s">
-        <v>9</v>
-      </c>
-      <c r="D233">
-        <v>1</v>
-      </c>
-      <c r="E233">
-        <v>5</v>
-      </c>
-      <c r="F233" t="s">
+      <c r="G233" t="s">
         <v>491</v>
-      </c>
-      <c r="G233" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="234" spans="1:7">
       <c r="A234" t="s">
+        <v>492</v>
+      </c>
+      <c r="B234" t="s">
+        <v>9</v>
+      </c>
+      <c r="F234" t="s">
+        <v>490</v>
+      </c>
+      <c r="G234" t="s">
         <v>493</v>
-      </c>
-      <c r="B234" t="s">
-        <v>13</v>
-      </c>
-      <c r="G234" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="235" spans="1:7">
       <c r="A235" t="s">
+        <v>494</v>
+      </c>
+      <c r="B235" t="s">
+        <v>9</v>
+      </c>
+      <c r="D235">
+        <v>1</v>
+      </c>
+      <c r="E235">
+        <v>5</v>
+      </c>
+      <c r="F235" t="s">
         <v>495</v>
-      </c>
-      <c r="B235" t="s">
-        <v>13</v>
       </c>
       <c r="G235" t="s">
         <v>496</v>
@@ -5746,16 +5773,7 @@
         <v>497</v>
       </c>
       <c r="B236" t="s">
-        <v>9</v>
-      </c>
-      <c r="D236">
-        <v>1</v>
-      </c>
-      <c r="E236">
-        <v>4</v>
-      </c>
-      <c r="F236" t="s">
-        <v>262</v>
+        <v>13</v>
       </c>
       <c r="G236" t="s">
         <v>498</v>
@@ -5768,12 +5786,6 @@
       <c r="B237" t="s">
         <v>13</v>
       </c>
-      <c r="D237">
-        <v>0</v>
-      </c>
-      <c r="E237">
-        <v>100</v>
-      </c>
       <c r="G237" t="s">
         <v>500</v>
       </c>
@@ -5783,13 +5795,16 @@
         <v>501</v>
       </c>
       <c r="B238" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D238">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E238">
-        <v>100</v>
+        <v>4</v>
+      </c>
+      <c r="F238" t="s">
+        <v>266</v>
       </c>
       <c r="G238" t="s">
         <v>502</v>
@@ -5802,6 +5817,12 @@
       <c r="B239" t="s">
         <v>13</v>
       </c>
+      <c r="D239">
+        <v>0</v>
+      </c>
+      <c r="E239">
+        <v>100</v>
+      </c>
       <c r="G239" t="s">
         <v>504</v>
       </c>
@@ -5830,12 +5851,6 @@
       <c r="B241" t="s">
         <v>13</v>
       </c>
-      <c r="D241">
-        <v>0</v>
-      </c>
-      <c r="E241">
-        <v>100</v>
-      </c>
       <c r="G241" t="s">
         <v>508</v>
       </c>
@@ -5845,16 +5860,13 @@
         <v>509</v>
       </c>
       <c r="B242" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D242">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E242">
-        <v>9</v>
-      </c>
-      <c r="F242" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G242" t="s">
         <v>510</v>
@@ -5882,13 +5894,16 @@
         <v>513</v>
       </c>
       <c r="B244" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D244">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E244">
-        <v>100</v>
+        <v>9</v>
+      </c>
+      <c r="F244" t="s">
+        <v>103</v>
       </c>
       <c r="G244" t="s">
         <v>514</v>
@@ -5901,6 +5916,12 @@
       <c r="B245" t="s">
         <v>13</v>
       </c>
+      <c r="D245">
+        <v>0</v>
+      </c>
+      <c r="E245">
+        <v>100</v>
+      </c>
       <c r="G245" t="s">
         <v>516</v>
       </c>
@@ -5927,47 +5948,44 @@
         <v>519</v>
       </c>
       <c r="B247" t="s">
-        <v>9</v>
-      </c>
-      <c r="D247">
-        <v>1</v>
-      </c>
-      <c r="E247">
-        <v>10</v>
-      </c>
-      <c r="F247" t="s">
+        <v>13</v>
+      </c>
+      <c r="G247" t="s">
         <v>520</v>
-      </c>
-      <c r="G247" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="248" spans="1:7">
       <c r="A248" t="s">
+        <v>521</v>
+      </c>
+      <c r="B248" t="s">
+        <v>13</v>
+      </c>
+      <c r="D248">
+        <v>0</v>
+      </c>
+      <c r="E248">
+        <v>100</v>
+      </c>
+      <c r="G248" t="s">
         <v>522</v>
-      </c>
-      <c r="B248" t="s">
-        <v>9</v>
-      </c>
-      <c r="F248" t="s">
-        <v>103</v>
-      </c>
-      <c r="G248" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="249" spans="1:7">
       <c r="A249" t="s">
+        <v>523</v>
+      </c>
+      <c r="B249" t="s">
+        <v>9</v>
+      </c>
+      <c r="D249">
+        <v>1</v>
+      </c>
+      <c r="E249">
+        <v>10</v>
+      </c>
+      <c r="F249" t="s">
         <v>524</v>
-      </c>
-      <c r="B249" t="s">
-        <v>13</v>
-      </c>
-      <c r="D249">
-        <v>0</v>
-      </c>
-      <c r="E249">
-        <v>100</v>
       </c>
       <c r="G249" t="s">
         <v>525</v>
@@ -5978,7 +5996,10 @@
         <v>526</v>
       </c>
       <c r="B250" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="F250" t="s">
+        <v>103</v>
       </c>
       <c r="G250" t="s">
         <v>527</v>
@@ -5991,6 +6012,12 @@
       <c r="B251" t="s">
         <v>13</v>
       </c>
+      <c r="D251">
+        <v>0</v>
+      </c>
+      <c r="E251">
+        <v>100</v>
+      </c>
       <c r="G251" t="s">
         <v>529</v>
       </c>
@@ -6055,16 +6082,7 @@
         <v>540</v>
       </c>
       <c r="B257" t="s">
-        <v>9</v>
-      </c>
-      <c r="D257">
-        <v>0</v>
-      </c>
-      <c r="E257">
-        <v>9</v>
-      </c>
-      <c r="F257" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G257" t="s">
         <v>541</v>
@@ -6077,12 +6095,6 @@
       <c r="B258" t="s">
         <v>13</v>
       </c>
-      <c r="D258">
-        <v>0</v>
-      </c>
-      <c r="E258">
-        <v>1000</v>
-      </c>
       <c r="G258" t="s">
         <v>543</v>
       </c>
@@ -6092,7 +6104,16 @@
         <v>544</v>
       </c>
       <c r="B259" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="D259">
+        <v>0</v>
+      </c>
+      <c r="E259">
+        <v>9</v>
+      </c>
+      <c r="F259" t="s">
+        <v>16</v>
       </c>
       <c r="G259" t="s">
         <v>545</v>
@@ -6131,16 +6152,13 @@
         <v>550</v>
       </c>
       <c r="B262" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D262">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E262">
-        <v>9</v>
-      </c>
-      <c r="F262" t="s">
-        <v>103</v>
+        <v>1000</v>
       </c>
       <c r="G262" t="s">
         <v>551</v>
@@ -6151,44 +6169,86 @@
         <v>552</v>
       </c>
       <c r="B263" t="s">
-        <v>9</v>
-      </c>
-      <c r="F263" t="s">
+        <v>13</v>
+      </c>
+      <c r="G263" t="s">
         <v>553</v>
-      </c>
-      <c r="G263" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="264" spans="1:7">
       <c r="A264" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B264" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D264">
         <v>1</v>
       </c>
       <c r="E264">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F264" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
       <c r="G264" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="265" spans="1:7">
       <c r="A265" t="s">
+        <v>556</v>
+      </c>
+      <c r="B265" t="s">
+        <v>9</v>
+      </c>
+      <c r="F265" t="s">
         <v>557</v>
-      </c>
-      <c r="B265" t="s">
-        <v>94</v>
       </c>
       <c r="G265" t="s">
         <v>558</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7">
+      <c r="A266" t="s">
+        <v>559</v>
+      </c>
+      <c r="B266" t="s">
+        <v>13</v>
+      </c>
+      <c r="D266">
+        <v>1</v>
+      </c>
+      <c r="E266">
+        <v>5</v>
+      </c>
+      <c r="F266" t="s">
+        <v>10</v>
+      </c>
+      <c r="G266" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7">
+      <c r="A267" t="s">
+        <v>561</v>
+      </c>
+      <c r="B267" t="s">
+        <v>94</v>
+      </c>
+      <c r="G267" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7">
+      <c r="A268" t="s">
+        <v>563</v>
+      </c>
+      <c r="B268" t="s">
+        <v>13</v>
+      </c>
+      <c r="G268" t="s">
+        <v>564</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update wheat trait ontology and properties
</commit_message>
<xml_diff>
--- a/ontology/triticum-props.xlsx
+++ b/ontology/triticum-props.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="575">
   <si>
     <t>trait_name</t>
   </si>
@@ -1709,6 +1709,36 @@
   </si>
   <si>
     <t>TRAIT: Grain area ::: METHOD: Grain Area Computation ::: SCALE: mm2</t>
+  </si>
+  <si>
+    <t>Spike wet weight - g</t>
+  </si>
+  <si>
+    <t>TRAIT: Spike wet weight ::: METHOD: Spike Wet Weight Measurement ::: SCALE: g</t>
+  </si>
+  <si>
+    <t>Plant stand - percent</t>
+  </si>
+  <si>
+    <t>TRAIT: Plant stand ::: METHOD: PlntStnd Estimation ::: SCALE: %</t>
+  </si>
+  <si>
+    <t>FHB Inoculation - Julian date (JD)</t>
+  </si>
+  <si>
+    <t>TRAIT: FHB inoculation ::: METHOD: FHB Inoculation Measurement ::: SCALE: Julian date (JD)</t>
+  </si>
+  <si>
+    <t>Canopy Cover - handheld - %</t>
+  </si>
+  <si>
+    <t>TRAIT: Canopy cover ::: METHOD: Canopy Cover HH Measurement ::: SCALE: %</t>
+  </si>
+  <si>
+    <t>Plot Damage - %</t>
+  </si>
+  <si>
+    <t>TRAIT: Plot damage ::: METHOD: Plot Damage Estimation ::: SCALE: %</t>
   </si>
 </sst>
 </file>
@@ -2040,7 +2070,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H268"/>
+  <dimension ref="A1:H273"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6251,6 +6281,79 @@
         <v>564</v>
       </c>
     </row>
+    <row r="269" spans="1:7">
+      <c r="A269" t="s">
+        <v>565</v>
+      </c>
+      <c r="B269" t="s">
+        <v>13</v>
+      </c>
+      <c r="G269" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="270" spans="1:7">
+      <c r="A270" t="s">
+        <v>567</v>
+      </c>
+      <c r="B270" t="s">
+        <v>13</v>
+      </c>
+      <c r="D270">
+        <v>0</v>
+      </c>
+      <c r="E270">
+        <v>100</v>
+      </c>
+      <c r="G270" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="271" spans="1:7">
+      <c r="A271" t="s">
+        <v>569</v>
+      </c>
+      <c r="B271" t="s">
+        <v>94</v>
+      </c>
+      <c r="G271" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7">
+      <c r="A272" t="s">
+        <v>571</v>
+      </c>
+      <c r="B272" t="s">
+        <v>13</v>
+      </c>
+      <c r="D272">
+        <v>0</v>
+      </c>
+      <c r="E272">
+        <v>100</v>
+      </c>
+      <c r="G272" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7">
+      <c r="A273" t="s">
+        <v>573</v>
+      </c>
+      <c r="B273" t="s">
+        <v>13</v>
+      </c>
+      <c r="D273">
+        <v>0</v>
+      </c>
+      <c r="E273">
+        <v>100</v>
+      </c>
+      <c r="G273" t="s">
+        <v>574</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update wheat trait ontology modify some scale min and max allowed values
</commit_message>
<xml_diff>
--- a/ontology/triticum-props.xlsx
+++ b/ontology/triticum-props.xlsx
@@ -2557,7 +2557,7 @@
         <v>13</v>
       </c>
       <c r="D29">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E29">
         <v>50000</v>
@@ -2574,10 +2574,10 @@
         <v>13</v>
       </c>
       <c r="D30">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="G30" t="s">
         <v>71</v>
@@ -2591,7 +2591,7 @@
         <v>13</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31">
         <v>30</v>
@@ -2653,7 +2653,7 @@
         <v>13</v>
       </c>
       <c r="D35">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E35">
         <v>70</v>
@@ -3001,7 +3001,7 @@
         <v>13</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E56">
         <v>50</v>
@@ -3233,7 +3233,7 @@
         <v>13</v>
       </c>
       <c r="D70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E70">
         <v>50</v>
@@ -3645,7 +3645,7 @@
         <v>13</v>
       </c>
       <c r="D96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96">
         <v>50</v>

</xml_diff>

<commit_message>
Update wheat trait ontology Add winter kill damage 0-9 trait
</commit_message>
<xml_diff>
--- a/ontology/triticum-props.xlsx
+++ b/ontology/triticum-props.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="581">
   <si>
     <t>trait_name</t>
   </si>
@@ -431,6 +431,12 @@
   </si>
   <si>
     <t>TRAIT: Stripe rust severity ::: METHOD: Rust severity Estimation ::: SCALE: %</t>
+  </si>
+  <si>
+    <t>Winter kill damage - 0-9 DAMAGE scale</t>
+  </si>
+  <si>
+    <t>TRAIT: Winter kill damage ::: METHOD: WKill Estimation ::: SCALE: 0-9 DAMAGE scale</t>
   </si>
   <si>
     <t>Winter kill damage - %</t>
@@ -2082,7 +2088,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H275"/>
+  <dimension ref="A1:H276"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3094,13 +3100,10 @@
         <v>139</v>
       </c>
       <c r="B62" t="s">
-        <v>13</v>
-      </c>
-      <c r="D62">
-        <v>0</v>
-      </c>
-      <c r="E62">
-        <v>100</v>
+        <v>9</v>
+      </c>
+      <c r="F62" t="s">
+        <v>16</v>
       </c>
       <c r="G62" t="s">
         <v>140</v>
@@ -3182,10 +3185,10 @@
         <v>13</v>
       </c>
       <c r="D67">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E67">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G67" t="s">
         <v>150</v>
@@ -3233,10 +3236,10 @@
         <v>13</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E70">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G70" t="s">
         <v>156</v>
@@ -3253,7 +3256,7 @@
         <v>0</v>
       </c>
       <c r="E71">
-        <v>1000</v>
+        <v>50</v>
       </c>
       <c r="G71" t="s">
         <v>158</v>
@@ -3270,7 +3273,7 @@
         <v>0</v>
       </c>
       <c r="E72">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="G72" t="s">
         <v>160</v>
@@ -3283,6 +3286,12 @@
       <c r="B73" t="s">
         <v>13</v>
       </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>200</v>
+      </c>
       <c r="G73" t="s">
         <v>162</v>
       </c>
@@ -3294,12 +3303,6 @@
       <c r="B74" t="s">
         <v>13</v>
       </c>
-      <c r="D74">
-        <v>0</v>
-      </c>
-      <c r="E74">
-        <v>90</v>
-      </c>
       <c r="G74" t="s">
         <v>164</v>
       </c>
@@ -3328,6 +3331,12 @@
       <c r="B76" t="s">
         <v>13</v>
       </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>90</v>
+      </c>
       <c r="G76" t="s">
         <v>168</v>
       </c>
@@ -3339,12 +3348,6 @@
       <c r="B77" t="s">
         <v>13</v>
       </c>
-      <c r="D77">
-        <v>0</v>
-      </c>
-      <c r="E77">
-        <v>90</v>
-      </c>
       <c r="G77" t="s">
         <v>170</v>
       </c>
@@ -3354,10 +3357,13 @@
         <v>171</v>
       </c>
       <c r="B78" t="s">
-        <v>9</v>
-      </c>
-      <c r="F78" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>90</v>
       </c>
       <c r="G78" t="s">
         <v>172</v>
@@ -3370,31 +3376,28 @@
       <c r="B79" t="s">
         <v>9</v>
       </c>
-      <c r="D79">
-        <v>1</v>
-      </c>
-      <c r="E79">
-        <v>6</v>
-      </c>
       <c r="F79" t="s">
+        <v>16</v>
+      </c>
+      <c r="G79" t="s">
         <v>174</v>
-      </c>
-      <c r="G79" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" t="s">
+        <v>175</v>
+      </c>
+      <c r="B80" t="s">
+        <v>9</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="E80">
+        <v>6</v>
+      </c>
+      <c r="F80" t="s">
         <v>176</v>
-      </c>
-      <c r="B80" t="s">
-        <v>13</v>
-      </c>
-      <c r="D80">
-        <v>0</v>
-      </c>
-      <c r="E80">
-        <v>100</v>
       </c>
       <c r="G80" t="s">
         <v>177</v>
@@ -3405,33 +3408,33 @@
         <v>178</v>
       </c>
       <c r="B81" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D81">
         <v>0</v>
       </c>
       <c r="E81">
-        <v>10</v>
-      </c>
-      <c r="F81" t="s">
+        <v>100</v>
+      </c>
+      <c r="G81" t="s">
         <v>179</v>
-      </c>
-      <c r="G81" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="82" spans="1:7">
       <c r="A82" t="s">
+        <v>180</v>
+      </c>
+      <c r="B82" t="s">
+        <v>9</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>10</v>
+      </c>
+      <c r="F82" t="s">
         <v>181</v>
-      </c>
-      <c r="B82" t="s">
-        <v>13</v>
-      </c>
-      <c r="D82">
-        <v>0</v>
-      </c>
-      <c r="E82">
-        <v>100</v>
       </c>
       <c r="G82" t="s">
         <v>182</v>
@@ -3442,16 +3445,13 @@
         <v>183</v>
       </c>
       <c r="B83" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E83">
-        <v>9</v>
-      </c>
-      <c r="F83" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G83" t="s">
         <v>184</v>
@@ -3462,13 +3462,16 @@
         <v>185</v>
       </c>
       <c r="B84" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E84">
-        <v>90</v>
+        <v>9</v>
+      </c>
+      <c r="F84" t="s">
+        <v>103</v>
       </c>
       <c r="G84" t="s">
         <v>186</v>
@@ -3485,7 +3488,7 @@
         <v>0</v>
       </c>
       <c r="E85">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="G85" t="s">
         <v>188</v>
@@ -3498,6 +3501,12 @@
       <c r="B86" t="s">
         <v>13</v>
       </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>100</v>
+      </c>
       <c r="G86" t="s">
         <v>190</v>
       </c>
@@ -3542,12 +3551,6 @@
       <c r="B90" t="s">
         <v>13</v>
       </c>
-      <c r="D90">
-        <v>0</v>
-      </c>
-      <c r="E90">
-        <v>90</v>
-      </c>
       <c r="G90" t="s">
         <v>198</v>
       </c>
@@ -3580,7 +3583,7 @@
         <v>0</v>
       </c>
       <c r="E92">
-        <v>200</v>
+        <v>90</v>
       </c>
       <c r="G92" t="s">
         <v>202</v>
@@ -3594,10 +3597,10 @@
         <v>13</v>
       </c>
       <c r="D93">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E93">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="G93" t="s">
         <v>204</v>
@@ -3611,10 +3614,10 @@
         <v>13</v>
       </c>
       <c r="D94">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E94">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="G94" t="s">
         <v>206</v>
@@ -3628,10 +3631,10 @@
         <v>13</v>
       </c>
       <c r="D95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E95">
-        <v>366</v>
+        <v>90</v>
       </c>
       <c r="G95" t="s">
         <v>208</v>
@@ -3645,10 +3648,10 @@
         <v>13</v>
       </c>
       <c r="D96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E96">
-        <v>50</v>
+        <v>366</v>
       </c>
       <c r="G96" t="s">
         <v>210</v>
@@ -3665,7 +3668,7 @@
         <v>0</v>
       </c>
       <c r="E97">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G97" t="s">
         <v>212</v>
@@ -3727,16 +3730,13 @@
         <v>219</v>
       </c>
       <c r="B101" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E101">
-        <v>9</v>
-      </c>
-      <c r="F101" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G101" t="s">
         <v>220</v>
@@ -3767,7 +3767,16 @@
         <v>223</v>
       </c>
       <c r="B103" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="D103">
+        <v>1</v>
+      </c>
+      <c r="E103">
+        <v>9</v>
+      </c>
+      <c r="F103" t="s">
+        <v>103</v>
       </c>
       <c r="G103" t="s">
         <v>224</v>
@@ -3778,16 +3787,7 @@
         <v>225</v>
       </c>
       <c r="B104" t="s">
-        <v>9</v>
-      </c>
-      <c r="D104">
-        <v>0</v>
-      </c>
-      <c r="E104">
-        <v>10</v>
-      </c>
-      <c r="F104" t="s">
-        <v>179</v>
+        <v>13</v>
       </c>
       <c r="G104" t="s">
         <v>226</v>
@@ -3800,8 +3800,14 @@
       <c r="B105" t="s">
         <v>9</v>
       </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105">
+        <v>10</v>
+      </c>
       <c r="F105" t="s">
-        <v>16</v>
+        <v>181</v>
       </c>
       <c r="G105" t="s">
         <v>228</v>
@@ -3812,13 +3818,10 @@
         <v>229</v>
       </c>
       <c r="B106" t="s">
-        <v>13</v>
-      </c>
-      <c r="D106">
-        <v>1</v>
-      </c>
-      <c r="E106">
-        <v>366</v>
+        <v>9</v>
+      </c>
+      <c r="F106" t="s">
+        <v>16</v>
       </c>
       <c r="G106" t="s">
         <v>230</v>
@@ -3832,10 +3835,10 @@
         <v>13</v>
       </c>
       <c r="D107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E107">
-        <v>200</v>
+        <v>366</v>
       </c>
       <c r="G107" t="s">
         <v>232</v>
@@ -3849,10 +3852,10 @@
         <v>13</v>
       </c>
       <c r="D108">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E108">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="G108" t="s">
         <v>234</v>
@@ -3863,13 +3866,13 @@
         <v>235</v>
       </c>
       <c r="B109" t="s">
-        <v>94</v>
+        <v>13</v>
       </c>
       <c r="D109">
+        <v>-1</v>
+      </c>
+      <c r="E109">
         <v>1</v>
-      </c>
-      <c r="E109">
-        <v>366</v>
       </c>
       <c r="G109" t="s">
         <v>236</v>
@@ -3880,13 +3883,13 @@
         <v>237</v>
       </c>
       <c r="B110" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="D110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E110">
-        <v>100</v>
+        <v>366</v>
       </c>
       <c r="G110" t="s">
         <v>238</v>
@@ -3988,7 +3991,7 @@
         <v>0</v>
       </c>
       <c r="E116">
-        <v>20000</v>
+        <v>100</v>
       </c>
       <c r="G116" t="s">
         <v>250</v>
@@ -3999,47 +4002,53 @@
         <v>251</v>
       </c>
       <c r="B117" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D117">
         <v>0</v>
       </c>
       <c r="E117">
-        <v>3</v>
-      </c>
-      <c r="F117" t="s">
+        <v>20000</v>
+      </c>
+      <c r="G117" t="s">
         <v>252</v>
-      </c>
-      <c r="G117" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="118" spans="1:7">
       <c r="A118" t="s">
+        <v>253</v>
+      </c>
+      <c r="B118" t="s">
+        <v>9</v>
+      </c>
+      <c r="D118">
+        <v>0</v>
+      </c>
+      <c r="E118">
+        <v>3</v>
+      </c>
+      <c r="F118" t="s">
         <v>254</v>
       </c>
-      <c r="B118" t="s">
-        <v>9</v>
-      </c>
-      <c r="D118">
-        <v>0</v>
-      </c>
-      <c r="E118">
-        <v>1</v>
-      </c>
-      <c r="F118" t="s">
+      <c r="G118" t="s">
         <v>255</v>
-      </c>
-      <c r="G118" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="119" spans="1:7">
       <c r="A119" t="s">
+        <v>256</v>
+      </c>
+      <c r="B119" t="s">
+        <v>9</v>
+      </c>
+      <c r="D119">
+        <v>0</v>
+      </c>
+      <c r="E119">
+        <v>1</v>
+      </c>
+      <c r="F119" t="s">
         <v>257</v>
-      </c>
-      <c r="B119" t="s">
-        <v>13</v>
       </c>
       <c r="G119" t="s">
         <v>258</v>
@@ -4074,12 +4083,6 @@
       <c r="B122" t="s">
         <v>13</v>
       </c>
-      <c r="D122">
-        <v>0</v>
-      </c>
-      <c r="E122">
-        <v>20000</v>
-      </c>
       <c r="G122" t="s">
         <v>264</v>
       </c>
@@ -4089,36 +4092,33 @@
         <v>265</v>
       </c>
       <c r="B123" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D123">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E123">
-        <v>4</v>
-      </c>
-      <c r="F123" t="s">
+        <v>20000</v>
+      </c>
+      <c r="G123" t="s">
         <v>266</v>
-      </c>
-      <c r="G123" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="124" spans="1:7">
       <c r="A124" t="s">
+        <v>267</v>
+      </c>
+      <c r="B124" t="s">
+        <v>9</v>
+      </c>
+      <c r="D124">
+        <v>1</v>
+      </c>
+      <c r="E124">
+        <v>4</v>
+      </c>
+      <c r="F124" t="s">
         <v>268</v>
-      </c>
-      <c r="B124" t="s">
-        <v>9</v>
-      </c>
-      <c r="D124">
-        <v>0</v>
-      </c>
-      <c r="E124">
-        <v>1</v>
-      </c>
-      <c r="F124" t="s">
-        <v>255</v>
       </c>
       <c r="G124" t="s">
         <v>269</v>
@@ -4131,8 +4131,14 @@
       <c r="B125" t="s">
         <v>9</v>
       </c>
+      <c r="D125">
+        <v>0</v>
+      </c>
+      <c r="E125">
+        <v>1</v>
+      </c>
       <c r="F125" t="s">
-        <v>16</v>
+        <v>257</v>
       </c>
       <c r="G125" t="s">
         <v>271</v>
@@ -4201,14 +4207,8 @@
       <c r="B130" t="s">
         <v>9</v>
       </c>
-      <c r="D130">
-        <v>1</v>
-      </c>
-      <c r="E130">
-        <v>9</v>
-      </c>
       <c r="F130" t="s">
-        <v>103</v>
+        <v>16</v>
       </c>
       <c r="G130" t="s">
         <v>281</v>
@@ -4219,13 +4219,16 @@
         <v>282</v>
       </c>
       <c r="B131" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D131">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E131">
-        <v>90</v>
+        <v>9</v>
+      </c>
+      <c r="F131" t="s">
+        <v>103</v>
       </c>
       <c r="G131" t="s">
         <v>283</v>
@@ -4239,10 +4242,10 @@
         <v>13</v>
       </c>
       <c r="D132">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E132">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="G132" t="s">
         <v>285</v>
@@ -4256,10 +4259,10 @@
         <v>13</v>
       </c>
       <c r="D133">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E133">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G133" t="s">
         <v>287</v>
@@ -4272,6 +4275,12 @@
       <c r="B134" t="s">
         <v>13</v>
       </c>
+      <c r="D134">
+        <v>0</v>
+      </c>
+      <c r="E134">
+        <v>100</v>
+      </c>
       <c r="G134" t="s">
         <v>289</v>
       </c>
@@ -4281,10 +4290,7 @@
         <v>290</v>
       </c>
       <c r="B135" t="s">
-        <v>9</v>
-      </c>
-      <c r="F135" t="s">
-        <v>135</v>
+        <v>13</v>
       </c>
       <c r="G135" t="s">
         <v>291</v>
@@ -4298,21 +4304,21 @@
         <v>9</v>
       </c>
       <c r="F136" t="s">
+        <v>135</v>
+      </c>
+      <c r="G136" t="s">
         <v>293</v>
-      </c>
-      <c r="G136" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="137" spans="1:7">
       <c r="A137" t="s">
+        <v>294</v>
+      </c>
+      <c r="B137" t="s">
+        <v>9</v>
+      </c>
+      <c r="F137" t="s">
         <v>295</v>
-      </c>
-      <c r="B137" t="s">
-        <v>9</v>
-      </c>
-      <c r="F137" t="s">
-        <v>135</v>
       </c>
       <c r="G137" t="s">
         <v>296</v>
@@ -4351,13 +4357,10 @@
         <v>301</v>
       </c>
       <c r="B140" t="s">
-        <v>13</v>
-      </c>
-      <c r="D140">
-        <v>0</v>
-      </c>
-      <c r="E140">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="F140" t="s">
+        <v>135</v>
       </c>
       <c r="G140" t="s">
         <v>302</v>
@@ -4374,7 +4377,7 @@
         <v>0</v>
       </c>
       <c r="E141">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="G141" t="s">
         <v>304</v>
@@ -4391,7 +4394,7 @@
         <v>0</v>
       </c>
       <c r="E142">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="G142" t="s">
         <v>306</v>
@@ -4419,13 +4422,13 @@
         <v>309</v>
       </c>
       <c r="B144" t="s">
-        <v>94</v>
+        <v>13</v>
       </c>
       <c r="D144">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E144">
-        <v>366</v>
+        <v>100</v>
       </c>
       <c r="G144" t="s">
         <v>310</v>
@@ -4453,13 +4456,13 @@
         <v>313</v>
       </c>
       <c r="B146" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="D146">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E146">
-        <v>90</v>
+        <v>366</v>
       </c>
       <c r="G146" t="s">
         <v>314</v>
@@ -4472,6 +4475,12 @@
       <c r="B147" t="s">
         <v>13</v>
       </c>
+      <c r="D147">
+        <v>0</v>
+      </c>
+      <c r="E147">
+        <v>90</v>
+      </c>
       <c r="G147" t="s">
         <v>316</v>
       </c>
@@ -4481,16 +4490,7 @@
         <v>317</v>
       </c>
       <c r="B148" t="s">
-        <v>9</v>
-      </c>
-      <c r="D148">
-        <v>1</v>
-      </c>
-      <c r="E148">
-        <v>6</v>
-      </c>
-      <c r="F148" t="s">
-        <v>174</v>
+        <v>13</v>
       </c>
       <c r="G148" t="s">
         <v>318</v>
@@ -4501,13 +4501,16 @@
         <v>319</v>
       </c>
       <c r="B149" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D149">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E149">
-        <v>100</v>
+        <v>6</v>
+      </c>
+      <c r="F149" t="s">
+        <v>176</v>
       </c>
       <c r="G149" t="s">
         <v>320</v>
@@ -4524,7 +4527,7 @@
         <v>0</v>
       </c>
       <c r="E150">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="G150" t="s">
         <v>322</v>
@@ -4552,16 +4555,13 @@
         <v>325</v>
       </c>
       <c r="B152" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D152">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E152">
-        <v>6</v>
-      </c>
-      <c r="F152" t="s">
-        <v>174</v>
+        <v>90</v>
       </c>
       <c r="G152" t="s">
         <v>326</v>
@@ -4572,13 +4572,16 @@
         <v>327</v>
       </c>
       <c r="B153" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D153">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E153">
-        <v>100</v>
+        <v>6</v>
+      </c>
+      <c r="F153" t="s">
+        <v>176</v>
       </c>
       <c r="G153" t="s">
         <v>328</v>
@@ -4595,7 +4598,7 @@
         <v>0</v>
       </c>
       <c r="E154">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="G154" t="s">
         <v>330</v>
@@ -4640,16 +4643,13 @@
         <v>335</v>
       </c>
       <c r="B157" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D157">
         <v>0</v>
       </c>
       <c r="E157">
-        <v>4</v>
-      </c>
-      <c r="F157" t="s">
-        <v>293</v>
+        <v>90</v>
       </c>
       <c r="G157" t="s">
         <v>336</v>
@@ -4660,13 +4660,16 @@
         <v>337</v>
       </c>
       <c r="B158" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D158">
         <v>0</v>
       </c>
       <c r="E158">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="F158" t="s">
+        <v>295</v>
       </c>
       <c r="G158" t="s">
         <v>338</v>
@@ -4677,16 +4680,13 @@
         <v>339</v>
       </c>
       <c r="B159" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D159">
         <v>0</v>
       </c>
       <c r="E159">
-        <v>10</v>
-      </c>
-      <c r="F159" t="s">
-        <v>179</v>
+        <v>1</v>
       </c>
       <c r="G159" t="s">
         <v>340</v>
@@ -4703,10 +4703,10 @@
         <v>0</v>
       </c>
       <c r="E160">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F160" t="s">
-        <v>255</v>
+        <v>181</v>
       </c>
       <c r="G160" t="s">
         <v>342</v>
@@ -4717,13 +4717,16 @@
         <v>343</v>
       </c>
       <c r="B161" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D161">
         <v>0</v>
       </c>
       <c r="E161">
-        <v>90</v>
+        <v>1</v>
+      </c>
+      <c r="F161" t="s">
+        <v>257</v>
       </c>
       <c r="G161" t="s">
         <v>344</v>
@@ -4736,6 +4739,12 @@
       <c r="B162" t="s">
         <v>13</v>
       </c>
+      <c r="D162">
+        <v>0</v>
+      </c>
+      <c r="E162">
+        <v>90</v>
+      </c>
       <c r="G162" t="s">
         <v>346</v>
       </c>
@@ -4747,12 +4756,6 @@
       <c r="B163" t="s">
         <v>13</v>
       </c>
-      <c r="D163">
-        <v>-1</v>
-      </c>
-      <c r="E163">
-        <v>1</v>
-      </c>
       <c r="G163" t="s">
         <v>348</v>
       </c>
@@ -4765,10 +4768,10 @@
         <v>13</v>
       </c>
       <c r="D164">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E164">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G164" t="s">
         <v>350</v>
@@ -4779,16 +4782,13 @@
         <v>351</v>
       </c>
       <c r="B165" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D165">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E165">
-        <v>5</v>
-      </c>
-      <c r="F165" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="G165" t="s">
         <v>352</v>
@@ -4801,8 +4801,14 @@
       <c r="B166" t="s">
         <v>9</v>
       </c>
+      <c r="D166">
+        <v>1</v>
+      </c>
+      <c r="E166">
+        <v>5</v>
+      </c>
       <c r="F166" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G166" t="s">
         <v>354</v>
@@ -4813,7 +4819,10 @@
         <v>355</v>
       </c>
       <c r="B167" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="F167" t="s">
+        <v>16</v>
       </c>
       <c r="G167" t="s">
         <v>356</v>
@@ -4824,10 +4833,7 @@
         <v>357</v>
       </c>
       <c r="B168" t="s">
-        <v>9</v>
-      </c>
-      <c r="F168" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G168" t="s">
         <v>358</v>
@@ -4882,14 +4888,8 @@
       <c r="B172" t="s">
         <v>9</v>
       </c>
-      <c r="D172">
-        <v>1</v>
-      </c>
-      <c r="E172">
-        <v>9</v>
-      </c>
       <c r="F172" t="s">
-        <v>103</v>
+        <v>16</v>
       </c>
       <c r="G172" t="s">
         <v>366</v>
@@ -4900,13 +4900,16 @@
         <v>367</v>
       </c>
       <c r="B173" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D173">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E173">
-        <v>100</v>
+        <v>9</v>
+      </c>
+      <c r="F173" t="s">
+        <v>103</v>
       </c>
       <c r="G173" t="s">
         <v>368</v>
@@ -4923,7 +4926,7 @@
         <v>0</v>
       </c>
       <c r="E174">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G174" t="s">
         <v>370</v>
@@ -4940,10 +4943,7 @@
         <v>0</v>
       </c>
       <c r="E175">
-        <v>9</v>
-      </c>
-      <c r="F175" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G175" t="s">
         <v>372</v>
@@ -5054,6 +5054,12 @@
         <v>383</v>
       </c>
       <c r="B181" t="s">
+        <v>13</v>
+      </c>
+      <c r="D181">
+        <v>0</v>
+      </c>
+      <c r="E181">
         <v>9</v>
       </c>
       <c r="F181" t="s">
@@ -5070,31 +5076,28 @@
       <c r="B182" t="s">
         <v>9</v>
       </c>
-      <c r="D182">
-        <v>5</v>
-      </c>
-      <c r="E182">
-        <v>25</v>
-      </c>
       <c r="F182" t="s">
+        <v>16</v>
+      </c>
+      <c r="G182" t="s">
         <v>386</v>
-      </c>
-      <c r="G182" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="183" spans="1:7">
       <c r="A183" t="s">
+        <v>387</v>
+      </c>
+      <c r="B183" t="s">
+        <v>9</v>
+      </c>
+      <c r="D183">
+        <v>5</v>
+      </c>
+      <c r="E183">
+        <v>25</v>
+      </c>
+      <c r="F183" t="s">
         <v>388</v>
-      </c>
-      <c r="B183" t="s">
-        <v>13</v>
-      </c>
-      <c r="D183">
-        <v>-1</v>
-      </c>
-      <c r="E183">
-        <v>1</v>
       </c>
       <c r="G183" t="s">
         <v>389</v>
@@ -5108,10 +5111,10 @@
         <v>13</v>
       </c>
       <c r="D184">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E184">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G184" t="s">
         <v>391</v>
@@ -5124,6 +5127,12 @@
       <c r="B185" t="s">
         <v>13</v>
       </c>
+      <c r="D185">
+        <v>0</v>
+      </c>
+      <c r="E185">
+        <v>100</v>
+      </c>
       <c r="G185" t="s">
         <v>393</v>
       </c>
@@ -5135,12 +5144,6 @@
       <c r="B186" t="s">
         <v>13</v>
       </c>
-      <c r="D186">
-        <v>0</v>
-      </c>
-      <c r="E186">
-        <v>100</v>
-      </c>
       <c r="G186" t="s">
         <v>395</v>
       </c>
@@ -5150,16 +5153,13 @@
         <v>396</v>
       </c>
       <c r="B187" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D187">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E187">
-        <v>9</v>
-      </c>
-      <c r="F187" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G187" t="s">
         <v>397</v>
@@ -5190,13 +5190,16 @@
         <v>400</v>
       </c>
       <c r="B189" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D189">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E189">
-        <v>100</v>
+        <v>9</v>
+      </c>
+      <c r="F189" t="s">
+        <v>103</v>
       </c>
       <c r="G189" t="s">
         <v>401</v>
@@ -5224,36 +5227,33 @@
         <v>404</v>
       </c>
       <c r="B191" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D191">
         <v>0</v>
       </c>
       <c r="E191">
-        <v>5</v>
-      </c>
-      <c r="F191" t="s">
+        <v>100</v>
+      </c>
+      <c r="G191" t="s">
         <v>405</v>
-      </c>
-      <c r="G191" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="192" spans="1:7">
       <c r="A192" t="s">
+        <v>406</v>
+      </c>
+      <c r="B192" t="s">
+        <v>9</v>
+      </c>
+      <c r="D192">
+        <v>0</v>
+      </c>
+      <c r="E192">
+        <v>5</v>
+      </c>
+      <c r="F192" t="s">
         <v>407</v>
-      </c>
-      <c r="B192" t="s">
-        <v>9</v>
-      </c>
-      <c r="D192">
-        <v>0</v>
-      </c>
-      <c r="E192">
-        <v>9</v>
-      </c>
-      <c r="F192" t="s">
-        <v>16</v>
       </c>
       <c r="G192" t="s">
         <v>408</v>
@@ -5266,8 +5266,14 @@
       <c r="B193" t="s">
         <v>9</v>
       </c>
+      <c r="D193">
+        <v>0</v>
+      </c>
+      <c r="E193">
+        <v>9</v>
+      </c>
       <c r="F193" t="s">
-        <v>135</v>
+        <v>16</v>
       </c>
       <c r="G193" t="s">
         <v>410</v>
@@ -5278,7 +5284,10 @@
         <v>411</v>
       </c>
       <c r="B194" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="F194" t="s">
+        <v>135</v>
       </c>
       <c r="G194" t="s">
         <v>412</v>
@@ -5335,12 +5344,6 @@
       <c r="B199" t="s">
         <v>13</v>
       </c>
-      <c r="D199">
-        <v>0</v>
-      </c>
-      <c r="E199">
-        <v>100</v>
-      </c>
       <c r="G199" t="s">
         <v>422</v>
       </c>
@@ -5350,10 +5353,13 @@
         <v>423</v>
       </c>
       <c r="B200" t="s">
-        <v>9</v>
-      </c>
-      <c r="F200" t="s">
-        <v>266</v>
+        <v>13</v>
+      </c>
+      <c r="D200">
+        <v>0</v>
+      </c>
+      <c r="E200">
+        <v>100</v>
       </c>
       <c r="G200" t="s">
         <v>424</v>
@@ -5367,7 +5373,7 @@
         <v>9</v>
       </c>
       <c r="F201" t="s">
-        <v>174</v>
+        <v>268</v>
       </c>
       <c r="G201" t="s">
         <v>426</v>
@@ -5381,7 +5387,7 @@
         <v>9</v>
       </c>
       <c r="F202" t="s">
-        <v>266</v>
+        <v>176</v>
       </c>
       <c r="G202" t="s">
         <v>428</v>
@@ -5392,16 +5398,10 @@
         <v>429</v>
       </c>
       <c r="B203" t="s">
-        <v>13</v>
-      </c>
-      <c r="D203">
-        <v>0</v>
-      </c>
-      <c r="E203">
         <v>9</v>
       </c>
       <c r="F203" t="s">
-        <v>16</v>
+        <v>268</v>
       </c>
       <c r="G203" t="s">
         <v>430</v>
@@ -5412,7 +5412,7 @@
         <v>431</v>
       </c>
       <c r="B204" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D204">
         <v>0</v>
@@ -5432,13 +5432,16 @@
         <v>433</v>
       </c>
       <c r="B205" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D205">
         <v>0</v>
       </c>
       <c r="E205">
-        <v>100</v>
+        <v>9</v>
+      </c>
+      <c r="F205" t="s">
+        <v>16</v>
       </c>
       <c r="G205" t="s">
         <v>434</v>
@@ -5449,16 +5452,13 @@
         <v>435</v>
       </c>
       <c r="B206" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D206">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E206">
-        <v>9</v>
-      </c>
-      <c r="F206" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G206" t="s">
         <v>436</v>
@@ -5469,13 +5469,16 @@
         <v>437</v>
       </c>
       <c r="B207" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D207">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E207">
-        <v>100</v>
+        <v>9</v>
+      </c>
+      <c r="F207" t="s">
+        <v>103</v>
       </c>
       <c r="G207" t="s">
         <v>438</v>
@@ -5492,7 +5495,7 @@
         <v>0</v>
       </c>
       <c r="E208">
-        <v>2.5</v>
+        <v>100</v>
       </c>
       <c r="G208" t="s">
         <v>440</v>
@@ -5505,6 +5508,12 @@
       <c r="B209" t="s">
         <v>13</v>
       </c>
+      <c r="D209">
+        <v>0</v>
+      </c>
+      <c r="E209">
+        <v>2.5</v>
+      </c>
       <c r="G209" t="s">
         <v>442</v>
       </c>
@@ -5516,12 +5525,6 @@
       <c r="B210" t="s">
         <v>13</v>
       </c>
-      <c r="D210">
-        <v>0</v>
-      </c>
-      <c r="E210">
-        <v>1000</v>
-      </c>
       <c r="G210" t="s">
         <v>444</v>
       </c>
@@ -5533,6 +5536,12 @@
       <c r="B211" t="s">
         <v>13</v>
       </c>
+      <c r="D211">
+        <v>0</v>
+      </c>
+      <c r="E211">
+        <v>1000</v>
+      </c>
       <c r="G211" t="s">
         <v>446</v>
       </c>
@@ -5544,12 +5553,6 @@
       <c r="B212" t="s">
         <v>13</v>
       </c>
-      <c r="D212">
-        <v>0</v>
-      </c>
-      <c r="E212">
-        <v>1000</v>
-      </c>
       <c r="G212" t="s">
         <v>448</v>
       </c>
@@ -5561,6 +5564,12 @@
       <c r="B213" t="s">
         <v>13</v>
       </c>
+      <c r="D213">
+        <v>0</v>
+      </c>
+      <c r="E213">
+        <v>1000</v>
+      </c>
       <c r="G213" t="s">
         <v>450</v>
       </c>
@@ -5572,12 +5581,6 @@
       <c r="B214" t="s">
         <v>13</v>
       </c>
-      <c r="D214">
-        <v>0</v>
-      </c>
-      <c r="E214">
-        <v>1000</v>
-      </c>
       <c r="G214" t="s">
         <v>452</v>
       </c>
@@ -5589,6 +5592,12 @@
       <c r="B215" t="s">
         <v>13</v>
       </c>
+      <c r="D215">
+        <v>0</v>
+      </c>
+      <c r="E215">
+        <v>1000</v>
+      </c>
       <c r="G215" t="s">
         <v>454</v>
       </c>
@@ -5600,12 +5609,6 @@
       <c r="B216" t="s">
         <v>13</v>
       </c>
-      <c r="D216">
-        <v>0</v>
-      </c>
-      <c r="E216">
-        <v>1000</v>
-      </c>
       <c r="G216" t="s">
         <v>456</v>
       </c>
@@ -5617,6 +5620,12 @@
       <c r="B217" t="s">
         <v>13</v>
       </c>
+      <c r="D217">
+        <v>0</v>
+      </c>
+      <c r="E217">
+        <v>1000</v>
+      </c>
       <c r="G217" t="s">
         <v>458</v>
       </c>
@@ -5639,12 +5648,6 @@
       <c r="B219" t="s">
         <v>13</v>
       </c>
-      <c r="D219">
-        <v>0</v>
-      </c>
-      <c r="E219">
-        <v>100</v>
-      </c>
       <c r="G219" t="s">
         <v>462</v>
       </c>
@@ -5656,6 +5659,12 @@
       <c r="B220" t="s">
         <v>13</v>
       </c>
+      <c r="D220">
+        <v>0</v>
+      </c>
+      <c r="E220">
+        <v>100</v>
+      </c>
       <c r="G220" t="s">
         <v>464</v>
       </c>
@@ -5676,10 +5685,7 @@
         <v>467</v>
       </c>
       <c r="B222" t="s">
-        <v>9</v>
-      </c>
-      <c r="F222" t="s">
-        <v>266</v>
+        <v>13</v>
       </c>
       <c r="G222" t="s">
         <v>468</v>
@@ -5690,7 +5696,10 @@
         <v>469</v>
       </c>
       <c r="B223" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="F223" t="s">
+        <v>268</v>
       </c>
       <c r="G223" t="s">
         <v>470</v>
@@ -5778,13 +5787,7 @@
         <v>485</v>
       </c>
       <c r="B231" t="s">
-        <v>94</v>
-      </c>
-      <c r="D231">
-        <v>1</v>
-      </c>
-      <c r="E231">
-        <v>366</v>
+        <v>13</v>
       </c>
       <c r="G231" t="s">
         <v>486</v>
@@ -5795,10 +5798,13 @@
         <v>487</v>
       </c>
       <c r="B232" t="s">
-        <v>9</v>
-      </c>
-      <c r="F232" t="s">
-        <v>10</v>
+        <v>94</v>
+      </c>
+      <c r="D232">
+        <v>1</v>
+      </c>
+      <c r="E232">
+        <v>366</v>
       </c>
       <c r="G232" t="s">
         <v>488</v>
@@ -5812,21 +5818,21 @@
         <v>9</v>
       </c>
       <c r="F233" t="s">
+        <v>10</v>
+      </c>
+      <c r="G233" t="s">
         <v>490</v>
-      </c>
-      <c r="G233" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="234" spans="1:7">
       <c r="A234" t="s">
+        <v>491</v>
+      </c>
+      <c r="B234" t="s">
+        <v>9</v>
+      </c>
+      <c r="F234" t="s">
         <v>492</v>
-      </c>
-      <c r="B234" t="s">
-        <v>9</v>
-      </c>
-      <c r="F234" t="s">
-        <v>490</v>
       </c>
       <c r="G234" t="s">
         <v>493</v>
@@ -5839,25 +5845,28 @@
       <c r="B235" t="s">
         <v>9</v>
       </c>
-      <c r="D235">
-        <v>1</v>
-      </c>
-      <c r="E235">
-        <v>5</v>
-      </c>
       <c r="F235" t="s">
+        <v>492</v>
+      </c>
+      <c r="G235" t="s">
         <v>495</v>
-      </c>
-      <c r="G235" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="236" spans="1:7">
       <c r="A236" t="s">
+        <v>496</v>
+      </c>
+      <c r="B236" t="s">
+        <v>9</v>
+      </c>
+      <c r="D236">
+        <v>1</v>
+      </c>
+      <c r="E236">
+        <v>5</v>
+      </c>
+      <c r="F236" t="s">
         <v>497</v>
-      </c>
-      <c r="B236" t="s">
-        <v>13</v>
       </c>
       <c r="G236" t="s">
         <v>498</v>
@@ -5879,16 +5888,7 @@
         <v>501</v>
       </c>
       <c r="B238" t="s">
-        <v>9</v>
-      </c>
-      <c r="D238">
-        <v>1</v>
-      </c>
-      <c r="E238">
-        <v>4</v>
-      </c>
-      <c r="F238" t="s">
-        <v>266</v>
+        <v>13</v>
       </c>
       <c r="G238" t="s">
         <v>502</v>
@@ -5899,13 +5899,16 @@
         <v>503</v>
       </c>
       <c r="B239" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D239">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E239">
-        <v>100</v>
+        <v>4</v>
+      </c>
+      <c r="F239" t="s">
+        <v>268</v>
       </c>
       <c r="G239" t="s">
         <v>504</v>
@@ -5935,6 +5938,12 @@
       <c r="B241" t="s">
         <v>13</v>
       </c>
+      <c r="D241">
+        <v>0</v>
+      </c>
+      <c r="E241">
+        <v>100</v>
+      </c>
       <c r="G241" t="s">
         <v>508</v>
       </c>
@@ -5946,12 +5955,6 @@
       <c r="B242" t="s">
         <v>13</v>
       </c>
-      <c r="D242">
-        <v>0</v>
-      </c>
-      <c r="E242">
-        <v>100</v>
-      </c>
       <c r="G242" t="s">
         <v>510</v>
       </c>
@@ -5978,16 +5981,13 @@
         <v>513</v>
       </c>
       <c r="B244" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D244">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E244">
-        <v>9</v>
-      </c>
-      <c r="F244" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G244" t="s">
         <v>514</v>
@@ -5998,13 +5998,16 @@
         <v>515</v>
       </c>
       <c r="B245" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D245">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E245">
-        <v>100</v>
+        <v>9</v>
+      </c>
+      <c r="F245" t="s">
+        <v>103</v>
       </c>
       <c r="G245" t="s">
         <v>516</v>
@@ -6034,6 +6037,12 @@
       <c r="B247" t="s">
         <v>13</v>
       </c>
+      <c r="D247">
+        <v>0</v>
+      </c>
+      <c r="E247">
+        <v>100</v>
+      </c>
       <c r="G247" t="s">
         <v>520</v>
       </c>
@@ -6045,12 +6054,6 @@
       <c r="B248" t="s">
         <v>13</v>
       </c>
-      <c r="D248">
-        <v>0</v>
-      </c>
-      <c r="E248">
-        <v>100</v>
-      </c>
       <c r="G248" t="s">
         <v>522</v>
       </c>
@@ -6060,30 +6063,33 @@
         <v>523</v>
       </c>
       <c r="B249" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D249">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E249">
-        <v>10</v>
-      </c>
-      <c r="F249" t="s">
+        <v>100</v>
+      </c>
+      <c r="G249" t="s">
         <v>524</v>
-      </c>
-      <c r="G249" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="250" spans="1:7">
       <c r="A250" t="s">
+        <v>525</v>
+      </c>
+      <c r="B250" t="s">
+        <v>9</v>
+      </c>
+      <c r="D250">
+        <v>1</v>
+      </c>
+      <c r="E250">
+        <v>10</v>
+      </c>
+      <c r="F250" t="s">
         <v>526</v>
-      </c>
-      <c r="B250" t="s">
-        <v>9</v>
-      </c>
-      <c r="F250" t="s">
-        <v>103</v>
       </c>
       <c r="G250" t="s">
         <v>527</v>
@@ -6094,13 +6100,10 @@
         <v>528</v>
       </c>
       <c r="B251" t="s">
-        <v>13</v>
-      </c>
-      <c r="D251">
-        <v>0</v>
-      </c>
-      <c r="E251">
-        <v>100</v>
+        <v>9</v>
+      </c>
+      <c r="F251" t="s">
+        <v>103</v>
       </c>
       <c r="G251" t="s">
         <v>529</v>
@@ -6113,6 +6116,12 @@
       <c r="B252" t="s">
         <v>13</v>
       </c>
+      <c r="D252">
+        <v>0</v>
+      </c>
+      <c r="E252">
+        <v>100</v>
+      </c>
       <c r="G252" t="s">
         <v>531</v>
       </c>
@@ -6188,16 +6197,7 @@
         <v>544</v>
       </c>
       <c r="B259" t="s">
-        <v>9</v>
-      </c>
-      <c r="D259">
-        <v>0</v>
-      </c>
-      <c r="E259">
-        <v>9</v>
-      </c>
-      <c r="F259" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G259" t="s">
         <v>545</v>
@@ -6208,13 +6208,16 @@
         <v>546</v>
       </c>
       <c r="B260" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D260">
         <v>0</v>
       </c>
       <c r="E260">
-        <v>1000</v>
+        <v>9</v>
+      </c>
+      <c r="F260" t="s">
+        <v>16</v>
       </c>
       <c r="G260" t="s">
         <v>547</v>
@@ -6227,6 +6230,12 @@
       <c r="B261" t="s">
         <v>13</v>
       </c>
+      <c r="D261">
+        <v>0</v>
+      </c>
+      <c r="E261">
+        <v>1000</v>
+      </c>
       <c r="G261" t="s">
         <v>549</v>
       </c>
@@ -6238,12 +6247,6 @@
       <c r="B262" t="s">
         <v>13</v>
       </c>
-      <c r="D262">
-        <v>0</v>
-      </c>
-      <c r="E262">
-        <v>1000</v>
-      </c>
       <c r="G262" t="s">
         <v>551</v>
       </c>
@@ -6255,6 +6258,12 @@
       <c r="B263" t="s">
         <v>13</v>
       </c>
+      <c r="D263">
+        <v>0</v>
+      </c>
+      <c r="E263">
+        <v>1000</v>
+      </c>
       <c r="G263" t="s">
         <v>553</v>
       </c>
@@ -6264,16 +6273,7 @@
         <v>554</v>
       </c>
       <c r="B264" t="s">
-        <v>9</v>
-      </c>
-      <c r="D264">
-        <v>1</v>
-      </c>
-      <c r="E264">
-        <v>9</v>
-      </c>
-      <c r="F264" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="G264" t="s">
         <v>555</v>
@@ -6286,28 +6286,28 @@
       <c r="B265" t="s">
         <v>9</v>
       </c>
+      <c r="D265">
+        <v>1</v>
+      </c>
+      <c r="E265">
+        <v>9</v>
+      </c>
       <c r="F265" t="s">
+        <v>103</v>
+      </c>
+      <c r="G265" t="s">
         <v>557</v>
-      </c>
-      <c r="G265" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="266" spans="1:7">
       <c r="A266" t="s">
+        <v>558</v>
+      </c>
+      <c r="B266" t="s">
+        <v>9</v>
+      </c>
+      <c r="F266" t="s">
         <v>559</v>
-      </c>
-      <c r="B266" t="s">
-        <v>13</v>
-      </c>
-      <c r="D266">
-        <v>1</v>
-      </c>
-      <c r="E266">
-        <v>5</v>
-      </c>
-      <c r="F266" t="s">
-        <v>10</v>
       </c>
       <c r="G266" t="s">
         <v>560</v>
@@ -6318,13 +6318,16 @@
         <v>561</v>
       </c>
       <c r="B267" t="s">
-        <v>94</v>
+        <v>13</v>
       </c>
       <c r="D267">
         <v>1</v>
       </c>
       <c r="E267">
-        <v>366</v>
+        <v>5</v>
+      </c>
+      <c r="F267" t="s">
+        <v>10</v>
       </c>
       <c r="G267" t="s">
         <v>562</v>
@@ -6335,7 +6338,13 @@
         <v>563</v>
       </c>
       <c r="B268" t="s">
-        <v>13</v>
+        <v>94</v>
+      </c>
+      <c r="D268">
+        <v>1</v>
+      </c>
+      <c r="E268">
+        <v>366</v>
       </c>
       <c r="G268" t="s">
         <v>564</v>
@@ -6359,12 +6368,6 @@
       <c r="B270" t="s">
         <v>13</v>
       </c>
-      <c r="D270">
-        <v>0</v>
-      </c>
-      <c r="E270">
-        <v>100</v>
-      </c>
       <c r="G270" t="s">
         <v>568</v>
       </c>
@@ -6374,13 +6377,13 @@
         <v>569</v>
       </c>
       <c r="B271" t="s">
-        <v>94</v>
+        <v>13</v>
       </c>
       <c r="D271">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E271">
-        <v>366</v>
+        <v>100</v>
       </c>
       <c r="G271" t="s">
         <v>570</v>
@@ -6391,13 +6394,13 @@
         <v>571</v>
       </c>
       <c r="B272" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="D272">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E272">
-        <v>100</v>
+        <v>366</v>
       </c>
       <c r="G272" t="s">
         <v>572</v>
@@ -6425,16 +6428,13 @@
         <v>575</v>
       </c>
       <c r="B274" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D274">
         <v>0</v>
       </c>
       <c r="E274">
-        <v>9</v>
-      </c>
-      <c r="F274" t="s">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="G274" t="s">
         <v>576</v>
@@ -6448,16 +6448,36 @@
         <v>9</v>
       </c>
       <c r="D275">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E275">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F275" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G275" t="s">
         <v>578</v>
+      </c>
+    </row>
+    <row r="276" spans="1:7">
+      <c r="A276" t="s">
+        <v>579</v>
+      </c>
+      <c r="B276" t="s">
+        <v>9</v>
+      </c>
+      <c r="D276">
+        <v>1</v>
+      </c>
+      <c r="E276">
+        <v>5</v>
+      </c>
+      <c r="F276" t="s">
+        <v>10</v>
+      </c>
+      <c r="G276" t="s">
+        <v>580</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update wheat trait ontology add dry forage content at Z85 trait
</commit_message>
<xml_diff>
--- a/ontology/triticum-props.xlsx
+++ b/ontology/triticum-props.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="583">
   <si>
     <t>trait_name</t>
   </si>
@@ -769,7 +769,7 @@
     <t>TRAIT: Forage starch content ::: METHOD: ForStr NIR Measurement ::: SCALE: %</t>
   </si>
   <si>
-    <t>Forage dry matter - kg/ha</t>
+    <t>Forage dry matter - at heading - kg/ha</t>
   </si>
   <si>
     <t>TRAIT: Forage dry matter ::: METHOD: ForgDM Computation ::: SCALE: kg/ha</t>
@@ -1757,6 +1757,12 @@
   </si>
   <si>
     <t>TRAIT: Winter Dormancy Release ::: METHOD: Winter Dormancy Release Estimation ::: SCALE: 1-5 WDR Response Scale</t>
+  </si>
+  <si>
+    <t>Forage dry matter - at soft dough - kg/ha</t>
+  </si>
+  <si>
+    <t>TRAIT: Forage dry matter ::: METHOD: ForgDM Computation Z85 ::: SCALE: kg/ha</t>
   </si>
 </sst>
 </file>
@@ -2088,7 +2094,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H276"/>
+  <dimension ref="A1:H277"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2679,7 +2685,7 @@
         <v>0</v>
       </c>
       <c r="E36">
-        <v>20000</v>
+        <v>35000</v>
       </c>
       <c r="G36" t="s">
         <v>83</v>
@@ -4008,7 +4014,7 @@
         <v>0</v>
       </c>
       <c r="E117">
-        <v>20000</v>
+        <v>35000</v>
       </c>
       <c r="G117" t="s">
         <v>252</v>
@@ -4098,7 +4104,7 @@
         <v>0</v>
       </c>
       <c r="E123">
-        <v>20000</v>
+        <v>35000</v>
       </c>
       <c r="G123" t="s">
         <v>266</v>
@@ -6478,6 +6484,23 @@
       </c>
       <c r="G276" t="s">
         <v>580</v>
+      </c>
+    </row>
+    <row r="277" spans="1:7">
+      <c r="A277" t="s">
+        <v>581</v>
+      </c>
+      <c r="B277" t="s">
+        <v>13</v>
+      </c>
+      <c r="D277">
+        <v>0</v>
+      </c>
+      <c r="E277">
+        <v>35000</v>
+      </c>
+      <c r="G277" t="s">
+        <v>582</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update wheat trait ontology add agronomic appearance trait
</commit_message>
<xml_diff>
--- a/ontology/triticum-props.xlsx
+++ b/ontology/triticum-props.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="586">
   <si>
     <t>trait_name</t>
   </si>
@@ -1763,6 +1763,15 @@
   </si>
   <si>
     <t>TRAIT: Forage dry matter ::: METHOD: ForgDM Computation Z85 ::: SCALE: kg/ha</t>
+  </si>
+  <si>
+    <t>Agronomic Appearance - 0-9 Scale</t>
+  </si>
+  <si>
+    <t>0/2/3/4/5/6/7/8/9</t>
+  </si>
+  <si>
+    <t>TRAIT: Agronomic appearance ::: METHOD: Agronomic Appearance Visual Estimation ::: SCALE: 0-9 Agronomic Appearance Scale</t>
   </si>
 </sst>
 </file>
@@ -2094,7 +2103,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H277"/>
+  <dimension ref="A1:H278"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6503,6 +6512,26 @@
         <v>582</v>
       </c>
     </row>
+    <row r="278" spans="1:7">
+      <c r="A278" t="s">
+        <v>583</v>
+      </c>
+      <c r="B278" t="s">
+        <v>9</v>
+      </c>
+      <c r="D278">
+        <v>0</v>
+      </c>
+      <c r="E278">
+        <v>9</v>
+      </c>
+      <c r="F278" t="s">
+        <v>584</v>
+      </c>
+      <c r="G278" t="s">
+        <v>585</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>